<commit_message>
fixed the column names in full_sample.xlsx
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duval/Documents/ULLYSES/CTTS_SAMPLE_UPDATES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23736F90-116B-8F45-8B35-D21885EDDB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4327BF-B02E-164E-95B1-61191AB1B491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="460" windowWidth="15020" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="475">
   <si>
-    <t>targets</t>
-  </si>
-  <si>
     <t>2MASS</t>
   </si>
   <si>
@@ -1087,21 +1084,12 @@
     <t>-39d08m51.8s</t>
   </si>
   <si>
-    <t>COS ORB</t>
-  </si>
-  <si>
-    <t>STIS ORB</t>
-  </si>
-  <si>
     <t>OLD COS orbs</t>
   </si>
   <si>
     <t>OLD STIS orbs</t>
   </si>
   <si>
-    <t>ORB</t>
-  </si>
-  <si>
     <t>DO</t>
   </si>
   <si>
@@ -1445,6 +1433,18 @@
   </si>
   <si>
     <t>13775|11616</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>COS orbs</t>
+  </si>
+  <si>
+    <t>STIS orbs</t>
+  </si>
+  <si>
+    <t>ORBS</t>
   </si>
 </sst>
 </file>
@@ -2711,9 +2711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W54" sqref="W54:W95"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2728,105 +2728,105 @@
   <sheetData>
     <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>471</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>356</v>
+      </c>
+      <c r="O1" t="s">
+        <v>354</v>
+      </c>
+      <c r="P1" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>357</v>
+      </c>
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>360</v>
-      </c>
-      <c r="O1" t="s">
-        <v>357</v>
-      </c>
-      <c r="P1" t="s">
-        <v>358</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>361</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
       <c r="T1" t="s">
-        <v>355</v>
+        <v>472</v>
       </c>
       <c r="U1" t="s">
-        <v>356</v>
+        <v>473</v>
       </c>
       <c r="V1" t="s">
-        <v>359</v>
+        <v>474</v>
       </c>
       <c r="W1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="X1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="Y1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="1">
         <v>440</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1">
         <v>0.56000000000000005</v>
@@ -2878,7 +2878,7 @@
         <v>16115</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -2886,26 +2886,26 @@
     </row>
     <row r="3" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1">
         <v>440</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1">
         <v>0.79</v>
@@ -2963,28 +2963,28 @@
     </row>
     <row r="4" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>440</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1">
         <v>0.92</v>
@@ -3042,28 +3042,28 @@
     </row>
     <row r="5" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G5" s="1">
         <v>385</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="1">
         <v>0.754</v>
@@ -3121,28 +3121,28 @@
     </row>
     <row r="6" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>385</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="1">
         <v>1.087</v>
@@ -3200,26 +3200,26 @@
     </row>
     <row r="7" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="1">
         <v>440</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" s="1">
         <v>0.77</v>
@@ -3277,26 +3277,26 @@
     </row>
     <row r="8" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G8" s="1">
         <v>330</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" s="1">
         <v>0.34</v>
@@ -3354,28 +3354,28 @@
     </row>
     <row r="9" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>385</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="1">
         <v>0.875</v>
@@ -3433,26 +3433,26 @@
     </row>
     <row r="10" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1">
         <v>440</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1">
         <v>0.77</v>
@@ -3510,26 +3510,26 @@
     </row>
     <row r="11" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="1">
         <v>440</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="1">
         <v>0.91</v>
@@ -3587,28 +3587,28 @@
     </row>
     <row r="12" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="1">
         <v>440</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" s="1">
         <v>0.35</v>
@@ -3666,26 +3666,26 @@
     </row>
     <row r="13" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="1">
         <v>440</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="1">
         <v>0.78</v>
@@ -3737,7 +3737,7 @@
         <v>16114</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="Y13">
         <v>2</v>
@@ -3745,26 +3745,26 @@
     </row>
     <row r="14" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="1">
         <v>330</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I14" s="1">
         <v>0.33</v>
@@ -3822,28 +3822,28 @@
     </row>
     <row r="15" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="G15" s="2">
         <v>46</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I15" s="2">
         <v>0.28999999999999998</v>
@@ -3896,28 +3896,28 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="G16" s="6">
         <v>150</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I16" s="6">
         <v>0.86</v>
@@ -3972,28 +3972,28 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>95</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G17" s="6">
         <v>150</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" s="6">
         <v>0.75</v>
@@ -4048,28 +4048,28 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" s="6">
         <v>150</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I18" s="6">
         <v>0.37</v>
@@ -4124,28 +4124,28 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>106</v>
-      </c>
       <c r="F19" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G19" s="6">
         <v>150</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I19" s="6">
         <v>0.2</v>
@@ -4200,26 +4200,26 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>109</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="F20" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G20" s="6">
         <v>150</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I20" s="6">
         <v>0.23</v>
@@ -4274,28 +4274,28 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="F21" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G21" s="6">
         <v>150</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I21" s="6">
         <v>0.42</v>
@@ -4350,28 +4350,28 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="F22" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="6">
         <v>150</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I22" s="6">
         <v>0.28999999999999998</v>
@@ -4426,28 +4426,28 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
         <v>124</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>125</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>126</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>127</v>
       </c>
-      <c r="E23" t="s">
-        <v>128</v>
-      </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G23">
         <v>150</v>
       </c>
       <c r="H23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I23">
         <v>0.3</v>
@@ -4498,28 +4498,28 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="G24" s="6">
         <v>160</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I24" s="6">
         <v>0.16</v>
@@ -4570,28 +4570,28 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="G25" s="6">
         <v>200</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I25" s="6">
         <v>0.47</v>
@@ -4646,28 +4646,28 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="G26" s="6">
         <v>150</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I26" s="6">
         <v>0.41</v>
@@ -4722,28 +4722,28 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>153</v>
-      </c>
       <c r="F27" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G27" s="6">
         <v>160</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I27" s="6">
         <v>0.17</v>
@@ -4794,28 +4794,28 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>158</v>
-      </c>
       <c r="F28" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G28" s="6">
         <v>150</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I28" s="6">
         <v>0.2</v>
@@ -4870,28 +4870,28 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" t="s">
         <v>159</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>160</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>161</v>
       </c>
-      <c r="E29" t="s">
-        <v>162</v>
-      </c>
       <c r="F29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G29">
         <v>160</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I29">
         <v>0.3</v>
@@ -4942,28 +4942,28 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>167</v>
-      </c>
       <c r="F30" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G30" s="6">
         <v>200</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I30" s="6">
         <v>0.16</v>
@@ -5018,28 +5018,28 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B31" t="s">
+        <v>167</v>
+      </c>
+      <c r="C31" t="s">
         <v>168</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>169</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>170</v>
       </c>
-      <c r="E31" t="s">
-        <v>171</v>
-      </c>
       <c r="F31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G31">
         <v>160</v>
       </c>
       <c r="H31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I31">
         <v>0.49</v>
@@ -5090,28 +5090,28 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" t="s">
         <v>173</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>174</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>175</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>176</v>
       </c>
-      <c r="E32" t="s">
-        <v>177</v>
-      </c>
       <c r="F32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G32">
         <v>200</v>
       </c>
       <c r="H32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I32">
         <v>0.44</v>
@@ -5162,25 +5162,25 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" t="s">
         <v>178</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>179</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>180</v>
       </c>
-      <c r="E33" t="s">
-        <v>181</v>
-      </c>
       <c r="F33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G33">
         <v>160</v>
       </c>
       <c r="H33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I33">
         <v>0.2</v>
@@ -5231,28 +5231,28 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="G34" s="3">
         <v>94</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I34" s="3">
         <v>0.15</v>
@@ -5305,28 +5305,28 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G35" s="3">
         <v>94</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I35" s="3">
         <v>0.15</v>
@@ -5379,28 +5379,28 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>194</v>
-      </c>
       <c r="F36" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G36" s="6">
         <v>94</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I36" s="6">
         <v>5.1999999999999998E-2</v>
@@ -5455,28 +5455,28 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G37" s="2">
         <v>94</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I37" s="2">
         <v>0.78</v>
@@ -5529,28 +5529,28 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G38" s="2">
         <v>94</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I38" s="2">
         <v>0.28999999999999998</v>
@@ -5603,28 +5603,28 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" t="s">
         <v>205</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>206</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>207</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>208</v>
       </c>
-      <c r="E39" t="s">
-        <v>209</v>
-      </c>
       <c r="F39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G39">
         <v>160</v>
       </c>
       <c r="H39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I39">
         <v>0.19</v>
@@ -5669,28 +5669,28 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>214</v>
-      </c>
       <c r="F40" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" s="6">
         <v>160</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I40" s="6">
         <v>0.14000000000000001</v>
@@ -5741,26 +5741,26 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>217</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>219</v>
-      </c>
       <c r="F41" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G41" s="6">
         <v>160</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I41" s="6">
         <v>1.25</v>
@@ -5815,28 +5815,28 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>225</v>
-      </c>
       <c r="F42" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G42" s="6">
         <v>160</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I42" s="6">
         <v>0.51</v>
@@ -5888,33 +5888,33 @@
         <v>16482</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>229</v>
-      </c>
       <c r="F43" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G43" s="6">
         <v>160</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I43" s="6">
         <v>0.19</v>
@@ -5969,28 +5969,28 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B44" t="s">
+        <v>229</v>
+      </c>
+      <c r="C44" t="s">
         <v>230</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>231</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>232</v>
       </c>
-      <c r="E44" t="s">
-        <v>233</v>
-      </c>
       <c r="F44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G44">
         <v>160</v>
       </c>
       <c r="H44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I44">
         <v>0.79</v>
@@ -6041,28 +6041,28 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>238</v>
-      </c>
       <c r="F45" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G45" s="6">
         <v>160</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I45" s="6">
         <v>0.25</v>
@@ -6117,28 +6117,28 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B46" t="s">
+        <v>238</v>
+      </c>
+      <c r="C46" t="s">
         <v>239</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>240</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>241</v>
       </c>
-      <c r="E46" t="s">
-        <v>242</v>
-      </c>
       <c r="F46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G46">
         <v>160</v>
       </c>
       <c r="H46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I46">
         <v>1.31</v>
@@ -6189,28 +6189,28 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B47" t="s">
+        <v>242</v>
+      </c>
+      <c r="C47" t="s">
         <v>243</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>244</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>245</v>
       </c>
-      <c r="E47" t="s">
-        <v>246</v>
-      </c>
       <c r="F47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G47">
         <v>160</v>
       </c>
       <c r="H47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I47">
         <v>0.78</v>
@@ -6261,28 +6261,28 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>246</v>
+      </c>
+      <c r="B48" t="s">
         <v>247</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>248</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>249</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>250</v>
       </c>
-      <c r="E48" t="s">
-        <v>251</v>
-      </c>
       <c r="F48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G48">
         <v>160</v>
       </c>
       <c r="H48" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I48">
         <v>2.08</v>
@@ -6333,28 +6333,28 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B49" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" t="s">
         <v>253</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>254</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>255</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>256</v>
-      </c>
-      <c r="F49" t="s">
-        <v>257</v>
       </c>
       <c r="G49">
         <v>114</v>
       </c>
       <c r="H49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I49">
         <v>0.9</v>
@@ -6405,28 +6405,28 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B50" t="s">
+        <v>257</v>
+      </c>
+      <c r="C50" t="s">
         <v>258</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>259</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>260</v>
       </c>
-      <c r="E50" t="s">
-        <v>261</v>
-      </c>
       <c r="F50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G50">
         <v>160</v>
       </c>
       <c r="H50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I50">
         <v>0.1</v>
@@ -6477,28 +6477,28 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" t="s">
         <v>263</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>264</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>265</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>266</v>
       </c>
-      <c r="E51" t="s">
-        <v>267</v>
-      </c>
       <c r="F51" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G51">
         <v>114</v>
       </c>
       <c r="H51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I51">
         <v>0.16</v>
@@ -6549,28 +6549,28 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" t="s">
         <v>268</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>269</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>270</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>271</v>
       </c>
-      <c r="E52" t="s">
-        <v>272</v>
-      </c>
       <c r="F52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G52">
         <v>200</v>
       </c>
       <c r="H52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I52">
         <v>0.22</v>
@@ -6621,28 +6621,28 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" t="s">
         <v>273</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>274</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>275</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>276</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>277</v>
-      </c>
-      <c r="F53" t="s">
-        <v>278</v>
       </c>
       <c r="G53">
         <v>130</v>
       </c>
       <c r="H53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I53">
         <v>0.93</v>
@@ -6693,25 +6693,25 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>278</v>
+      </c>
+      <c r="B54" t="s">
         <v>279</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>280</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>281</v>
       </c>
-      <c r="E54" t="s">
-        <v>282</v>
-      </c>
       <c r="F54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G54">
         <v>150</v>
       </c>
       <c r="H54" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I54">
         <v>0.16</v>
@@ -6762,28 +6762,28 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>282</v>
+      </c>
+      <c r="B55" t="s">
         <v>283</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>284</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>285</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>286</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>287</v>
-      </c>
-      <c r="F55" t="s">
-        <v>288</v>
       </c>
       <c r="G55">
         <v>150</v>
       </c>
       <c r="H55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I55">
         <v>0.5</v>
@@ -6834,28 +6834,28 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>288</v>
+      </c>
+      <c r="B56" t="s">
         <v>289</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>290</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>291</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>292</v>
       </c>
-      <c r="E56" t="s">
-        <v>293</v>
-      </c>
       <c r="F56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G56">
         <v>150</v>
       </c>
       <c r="H56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I56">
         <v>0.95</v>
@@ -6906,28 +6906,28 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>294</v>
+      </c>
+      <c r="B57" t="s">
         <v>295</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>296</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>297</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>298</v>
       </c>
-      <c r="E57" t="s">
-        <v>299</v>
-      </c>
       <c r="F57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G57">
         <v>200</v>
       </c>
       <c r="H57" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I57">
         <v>0.21</v>
@@ -6978,28 +6978,28 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>300</v>
+      </c>
+      <c r="B58" t="s">
         <v>301</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>302</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>303</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>304</v>
       </c>
-      <c r="E58" t="s">
-        <v>305</v>
-      </c>
       <c r="F58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G58">
         <v>200</v>
       </c>
       <c r="H58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I58">
         <v>0.23</v>
@@ -7050,28 +7050,28 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>305</v>
+      </c>
+      <c r="B59" t="s">
         <v>306</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>307</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>308</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>309</v>
       </c>
-      <c r="E59" t="s">
-        <v>310</v>
-      </c>
       <c r="F59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G59">
         <v>200</v>
       </c>
       <c r="H59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I59">
         <v>0.26</v>
@@ -7122,28 +7122,28 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>310</v>
+      </c>
+      <c r="B60" t="s">
         <v>311</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>312</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>313</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>314</v>
       </c>
-      <c r="E60" t="s">
-        <v>315</v>
-      </c>
       <c r="F60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G60">
         <v>200</v>
       </c>
       <c r="H60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I60">
         <v>0.23</v>
@@ -7194,28 +7194,28 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>315</v>
+      </c>
+      <c r="B61" t="s">
         <v>316</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>317</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>318</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>319</v>
       </c>
-      <c r="E61" t="s">
-        <v>320</v>
-      </c>
       <c r="F61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G61">
         <v>200</v>
       </c>
       <c r="H61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I61">
         <v>0.16</v>
@@ -7266,28 +7266,28 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>320</v>
+      </c>
+      <c r="B62" t="s">
         <v>321</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>322</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>323</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>324</v>
       </c>
-      <c r="E62" t="s">
-        <v>325</v>
-      </c>
       <c r="F62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G62">
         <v>200</v>
       </c>
       <c r="H62" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I62">
         <v>0.7</v>
@@ -7338,28 +7338,28 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>325</v>
+      </c>
+      <c r="B63" t="s">
         <v>326</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>327</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>328</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>329</v>
       </c>
-      <c r="E63" t="s">
-        <v>330</v>
-      </c>
       <c r="F63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G63">
         <v>200</v>
       </c>
       <c r="H63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I63">
         <v>0.17</v>
@@ -7410,25 +7410,25 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>330</v>
+      </c>
+      <c r="B64" t="s">
         <v>331</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>332</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>333</v>
       </c>
-      <c r="E64" t="s">
-        <v>334</v>
-      </c>
       <c r="F64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G64">
         <v>130</v>
       </c>
       <c r="H64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I64">
         <v>1.04</v>
@@ -7479,28 +7479,28 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>334</v>
+      </c>
+      <c r="B65" t="s">
         <v>335</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>336</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>337</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>338</v>
       </c>
-      <c r="E65" t="s">
-        <v>339</v>
-      </c>
       <c r="F65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G65">
         <v>150</v>
       </c>
       <c r="H65" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I65">
         <v>0.79</v>
@@ -7551,28 +7551,28 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>339</v>
+      </c>
+      <c r="B66" t="s">
         <v>340</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>341</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>342</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>343</v>
       </c>
-      <c r="E66" t="s">
-        <v>344</v>
-      </c>
       <c r="F66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G66">
         <v>200</v>
       </c>
       <c r="H66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I66">
         <v>0.16</v>
@@ -7623,28 +7623,28 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>344</v>
+      </c>
+      <c r="B67" t="s">
         <v>345</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>346</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>347</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>348</v>
       </c>
-      <c r="E67" t="s">
-        <v>349</v>
-      </c>
       <c r="F67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G67">
         <v>200</v>
       </c>
       <c r="H67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I67">
         <v>0.22</v>
@@ -7695,28 +7695,28 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68" t="s">
         <v>350</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>351</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>352</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>353</v>
       </c>
-      <c r="E68" t="s">
-        <v>354</v>
-      </c>
       <c r="F68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G68">
         <v>200</v>
       </c>
       <c r="H68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I68">
         <v>0.19</v>
@@ -7767,28 +7767,28 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B69" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" t="s">
         <v>33</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>34</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>35</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>36</v>
-      </c>
-      <c r="F69" t="s">
-        <v>37</v>
       </c>
       <c r="G69">
         <v>385</v>
       </c>
       <c r="H69" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I69">
         <v>0.754</v>
@@ -7839,28 +7839,28 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B70" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C70" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D70" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F70" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G70">
         <v>140</v>
       </c>
       <c r="H70" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I70">
         <v>1.4</v>
@@ -7904,28 +7904,28 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B71" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C71" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D71" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E71" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F71" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G71">
         <v>94</v>
       </c>
       <c r="H71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I71">
         <v>0.3</v>
@@ -7969,28 +7969,28 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>389</v>
+      </c>
+      <c r="B72" t="s">
+        <v>390</v>
+      </c>
+      <c r="C72" t="s">
+        <v>391</v>
+      </c>
+      <c r="D72" t="s">
+        <v>392</v>
+      </c>
+      <c r="E72" t="s">
         <v>393</v>
       </c>
-      <c r="B72" t="s">
-        <v>394</v>
-      </c>
-      <c r="C72" t="s">
-        <v>395</v>
-      </c>
-      <c r="D72" t="s">
-        <v>396</v>
-      </c>
-      <c r="E72" t="s">
-        <v>397</v>
-      </c>
       <c r="F72" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G72">
         <v>94</v>
       </c>
       <c r="H72" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I72">
         <v>0.2</v>
@@ -8035,10 +8035,10 @@
         <v>0</v>
       </c>
       <c r="W72" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="X72" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="Y72">
         <v>3</v>
@@ -8046,28 +8046,28 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>395</v>
+      </c>
+      <c r="B73" t="s">
+        <v>396</v>
+      </c>
+      <c r="C73" t="s">
+        <v>397</v>
+      </c>
+      <c r="D73" t="s">
+        <v>398</v>
+      </c>
+      <c r="E73" t="s">
         <v>399</v>
       </c>
-      <c r="B73" t="s">
-        <v>400</v>
-      </c>
-      <c r="C73" t="s">
-        <v>401</v>
-      </c>
-      <c r="D73" t="s">
-        <v>402</v>
-      </c>
-      <c r="E73" t="s">
-        <v>403</v>
-      </c>
       <c r="F73" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G73">
         <v>94</v>
       </c>
       <c r="H73" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I73">
         <v>0.75</v>
@@ -8115,7 +8115,7 @@
         <v>11616</v>
       </c>
       <c r="X73" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="Y73">
         <v>3</v>
@@ -8123,28 +8123,28 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>400</v>
+      </c>
+      <c r="B74" t="s">
+        <v>401</v>
+      </c>
+      <c r="C74" t="s">
+        <v>402</v>
+      </c>
+      <c r="D74" t="s">
+        <v>403</v>
+      </c>
+      <c r="E74" t="s">
         <v>404</v>
       </c>
-      <c r="B74" t="s">
-        <v>405</v>
-      </c>
-      <c r="C74" t="s">
-        <v>406</v>
-      </c>
-      <c r="D74" t="s">
-        <v>407</v>
-      </c>
-      <c r="E74" t="s">
-        <v>408</v>
-      </c>
       <c r="F74" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G74">
         <v>94</v>
       </c>
       <c r="H74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I74">
         <v>0.83</v>
@@ -8192,7 +8192,7 @@
         <v>11616</v>
       </c>
       <c r="X74" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="Y74">
         <v>3</v>
@@ -8200,28 +8200,28 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>407</v>
+      </c>
+      <c r="B75" t="s">
+        <v>408</v>
+      </c>
+      <c r="C75" t="s">
+        <v>409</v>
+      </c>
+      <c r="D75" t="s">
+        <v>410</v>
+      </c>
+      <c r="E75" t="s">
         <v>411</v>
       </c>
-      <c r="B75" t="s">
+      <c r="F75" t="s">
         <v>412</v>
-      </c>
-      <c r="C75" t="s">
-        <v>413</v>
-      </c>
-      <c r="D75" t="s">
-        <v>414</v>
-      </c>
-      <c r="E75" t="s">
-        <v>415</v>
-      </c>
-      <c r="F75" t="s">
-        <v>416</v>
       </c>
       <c r="G75">
         <v>150</v>
       </c>
       <c r="H75" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="I75">
         <v>1.06</v>
@@ -8269,7 +8269,7 @@
         <v>14604</v>
       </c>
       <c r="X75" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="Y75">
         <v>3</v>
@@ -8277,28 +8277,28 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>414</v>
+      </c>
+      <c r="B76" t="s">
+        <v>415</v>
+      </c>
+      <c r="C76" t="s">
+        <v>416</v>
+      </c>
+      <c r="D76" t="s">
+        <v>417</v>
+      </c>
+      <c r="E76" t="s">
         <v>418</v>
       </c>
-      <c r="B76" t="s">
-        <v>419</v>
-      </c>
-      <c r="C76" t="s">
-        <v>420</v>
-      </c>
-      <c r="D76" t="s">
-        <v>421</v>
-      </c>
-      <c r="E76" t="s">
-        <v>422</v>
-      </c>
       <c r="F76" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="G76">
         <v>150</v>
       </c>
       <c r="H76" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="I76">
         <v>1.4</v>
@@ -8343,10 +8343,10 @@
         <v>0</v>
       </c>
       <c r="W76" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="X76" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="Y76">
         <v>3</v>
@@ -8354,28 +8354,28 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>420</v>
+      </c>
+      <c r="B77" t="s">
+        <v>421</v>
+      </c>
+      <c r="C77" t="s">
+        <v>422</v>
+      </c>
+      <c r="D77" t="s">
+        <v>423</v>
+      </c>
+      <c r="E77" t="s">
         <v>424</v>
       </c>
-      <c r="B77" t="s">
-        <v>425</v>
-      </c>
-      <c r="C77" t="s">
-        <v>426</v>
-      </c>
-      <c r="D77" t="s">
-        <v>427</v>
-      </c>
-      <c r="E77" t="s">
-        <v>428</v>
-      </c>
       <c r="F77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G77">
         <v>200</v>
       </c>
       <c r="H77" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="I77">
         <v>1.4</v>
@@ -8423,7 +8423,7 @@
         <v>14604</v>
       </c>
       <c r="X77" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="Y77">
         <v>3</v>
@@ -8431,28 +8431,28 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>425</v>
+      </c>
+      <c r="B78" t="s">
+        <v>426</v>
+      </c>
+      <c r="C78" t="s">
+        <v>427</v>
+      </c>
+      <c r="D78" t="s">
+        <v>428</v>
+      </c>
+      <c r="E78" t="s">
         <v>429</v>
       </c>
-      <c r="B78" t="s">
+      <c r="F78" t="s">
         <v>430</v>
-      </c>
-      <c r="C78" t="s">
-        <v>431</v>
-      </c>
-      <c r="D78" t="s">
-        <v>432</v>
-      </c>
-      <c r="E78" t="s">
-        <v>433</v>
-      </c>
-      <c r="F78" t="s">
-        <v>434</v>
       </c>
       <c r="G78">
         <v>150</v>
       </c>
       <c r="H78" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="I78">
         <v>1.4</v>
@@ -8497,10 +8497,10 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="X78" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="Y78">
         <v>3</v>
@@ -8508,28 +8508,28 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>434</v>
+      </c>
+      <c r="B79" t="s">
+        <v>435</v>
+      </c>
+      <c r="C79" t="s">
+        <v>436</v>
+      </c>
+      <c r="D79" t="s">
+        <v>437</v>
+      </c>
+      <c r="E79" t="s">
         <v>438</v>
       </c>
-      <c r="B79" t="s">
-        <v>439</v>
-      </c>
-      <c r="C79" t="s">
-        <v>440</v>
-      </c>
-      <c r="D79" t="s">
-        <v>441</v>
-      </c>
-      <c r="E79" t="s">
-        <v>442</v>
-      </c>
       <c r="F79" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G79">
         <v>114</v>
       </c>
       <c r="H79" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="I79">
         <v>2.5299999999999998</v>
@@ -8574,10 +8574,10 @@
         <v>0</v>
       </c>
       <c r="W79" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="X79" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="Y79">
         <v>3</v>
@@ -8585,28 +8585,28 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>442</v>
+      </c>
+      <c r="B80" t="s">
+        <v>443</v>
+      </c>
+      <c r="C80" t="s">
+        <v>444</v>
+      </c>
+      <c r="D80" t="s">
+        <v>445</v>
+      </c>
+      <c r="E80" t="s">
         <v>446</v>
       </c>
-      <c r="B80" t="s">
-        <v>447</v>
-      </c>
-      <c r="C80" t="s">
-        <v>448</v>
-      </c>
-      <c r="D80" t="s">
-        <v>449</v>
-      </c>
-      <c r="E80" t="s">
-        <v>450</v>
-      </c>
       <c r="F80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G80">
         <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="I80">
         <v>0.67</v>
@@ -8654,7 +8654,7 @@
         <v>14193</v>
       </c>
       <c r="X80" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="Y80">
         <v>3</v>
@@ -8662,28 +8662,28 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>448</v>
+      </c>
+      <c r="B81" t="s">
+        <v>449</v>
+      </c>
+      <c r="C81" t="s">
+        <v>450</v>
+      </c>
+      <c r="D81" t="s">
+        <v>451</v>
+      </c>
+      <c r="E81" t="s">
         <v>452</v>
       </c>
-      <c r="B81" t="s">
-        <v>453</v>
-      </c>
-      <c r="C81" t="s">
-        <v>454</v>
-      </c>
-      <c r="D81" t="s">
-        <v>455</v>
-      </c>
-      <c r="E81" t="s">
-        <v>456</v>
-      </c>
       <c r="F81" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G81">
         <v>160</v>
       </c>
       <c r="H81" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="I81">
         <v>1.4</v>
@@ -8728,10 +8728,10 @@
         <v>0</v>
       </c>
       <c r="W81" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="X81" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="Y81">
         <v>3</v>
@@ -8739,28 +8739,28 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B82" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C82" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D82" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E82" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F82" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G82">
         <v>160</v>
       </c>
       <c r="H82" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="I82">
         <v>1.62</v>
@@ -8808,10 +8808,10 @@
         <v>11616</v>
       </c>
       <c r="X82" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="Y82" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the orbits for RECX5 and 9 to reflect the fact that they will be observed with STIS/G140L and G130M/1222 based on SAC input
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4327BF-B02E-164E-95B1-61191AB1B491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06100B45-FFA3-D844-BFAC-E6D8971A9204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="460" windowWidth="15020" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2180" yWindow="460" windowWidth="27700" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -2712,8 +2712,8 @@
   <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X1" sqref="X1"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5289,12 +5289,10 @@
         <v>0.27</v>
       </c>
       <c r="T34" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U34" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V34" s="3">
         <f>Q34</f>
@@ -5363,12 +5361,10 @@
         <v>0.27</v>
       </c>
       <c r="T35" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U35" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V35" s="3">
         <f t="shared" ref="V35:V36" si="5">Q35</f>

</xml_diff>

<commit_message>
fixed coordinates of RECX 6 (typo)
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06100B45-FFA3-D844-BFAC-E6D8971A9204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE9F41D-5F07-7A45-9EBD-8869C6F42E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="460" windowWidth="27700" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2720" yWindow="460" windowWidth="17880" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -1108,9 +1108,6 @@
     <t>08h42m38.78s</t>
   </si>
   <si>
-    <t>-78d54m42,74s</t>
-  </si>
-  <si>
     <t>Eta Cha</t>
   </si>
   <si>
@@ -1445,6 +1442,9 @@
   </si>
   <si>
     <t>ORBS</t>
+  </si>
+  <si>
+    <t>-78d54m42.74s</t>
   </si>
 </sst>
 </file>
@@ -2711,24 +2711,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X34" sqref="X34"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="15" max="15" width="3.1640625" customWidth="1"/>
     <col min="16" max="17" width="12.5" customWidth="1"/>
     <col min="18" max="18" width="14.5" customWidth="1"/>
     <col min="19" max="19" width="18.33203125" customWidth="1"/>
-    <col min="24" max="24" width="59.5" customWidth="1"/>
+    <col min="24" max="24" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2785,22 +2786,22 @@
         <v>13</v>
       </c>
       <c r="T1" t="s">
+        <v>471</v>
+      </c>
+      <c r="U1" t="s">
         <v>472</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>473</v>
       </c>
-      <c r="V1" t="s">
-        <v>474</v>
-      </c>
       <c r="W1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="X1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Y1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2878,7 +2879,7 @@
         <v>16115</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -3042,7 +3043,7 @@
     </row>
     <row r="5" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -3121,7 +3122,7 @@
     </row>
     <row r="6" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>38</v>
@@ -3354,7 +3355,7 @@
     </row>
     <row r="9" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>53</v>
@@ -3737,7 +3738,7 @@
         <v>16114</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="Y13">
         <v>2</v>
@@ -3822,7 +3823,7 @@
     </row>
     <row r="15" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>79</v>
@@ -4722,7 +4723,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>149</v>
@@ -4870,7 +4871,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B29" t="s">
         <v>158</v>
@@ -5018,7 +5019,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B31" t="s">
         <v>167</v>
@@ -5231,7 +5232,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>181</v>
@@ -5303,7 +5304,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>186</v>
@@ -5375,7 +5376,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>190</v>
@@ -5451,7 +5452,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>195</v>
@@ -5525,7 +5526,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>199</v>
@@ -5884,12 +5885,12 @@
         <v>16482</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>225</v>
@@ -5965,7 +5966,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B44" t="s">
         <v>229</v>
@@ -6113,7 +6114,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B46" t="s">
         <v>238</v>
@@ -6185,7 +6186,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B47" t="s">
         <v>242</v>
@@ -6329,7 +6330,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B49" t="s">
         <v>252</v>
@@ -6401,7 +6402,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B50" t="s">
         <v>257</v>
@@ -7763,7 +7764,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B69" t="s">
         <v>32</v>
@@ -7835,13 +7836,13 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B70" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C70" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D70" t="s">
         <v>358</v>
@@ -7900,22 +7901,22 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B71" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C71" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D71" t="s">
         <v>361</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="F71" t="s">
         <v>362</v>
-      </c>
-      <c r="F71" t="s">
-        <v>363</v>
       </c>
       <c r="G71">
         <v>94</v>
@@ -7965,28 +7966,28 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>388</v>
+      </c>
+      <c r="B72" t="s">
         <v>389</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>390</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>391</v>
       </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>392</v>
       </c>
-      <c r="E72" t="s">
-        <v>393</v>
-      </c>
       <c r="F72" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G72">
         <v>94</v>
       </c>
       <c r="H72" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I72">
         <v>0.2</v>
@@ -8031,10 +8032,10 @@
         <v>0</v>
       </c>
       <c r="W72" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="X72" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y72">
         <v>3</v>
@@ -8042,22 +8043,22 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>394</v>
+      </c>
+      <c r="B73" t="s">
         <v>395</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>396</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>397</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>398</v>
       </c>
-      <c r="E73" t="s">
-        <v>399</v>
-      </c>
       <c r="F73" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G73">
         <v>94</v>
@@ -8111,7 +8112,7 @@
         <v>11616</v>
       </c>
       <c r="X73" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y73">
         <v>3</v>
@@ -8119,22 +8120,22 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>399</v>
+      </c>
+      <c r="B74" t="s">
         <v>400</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>401</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>402</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>403</v>
       </c>
-      <c r="E74" t="s">
-        <v>404</v>
-      </c>
       <c r="F74" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G74">
         <v>94</v>
@@ -8188,7 +8189,7 @@
         <v>11616</v>
       </c>
       <c r="X74" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y74">
         <v>3</v>
@@ -8196,28 +8197,28 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>406</v>
+      </c>
+      <c r="B75" t="s">
         <v>407</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>408</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>409</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>410</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>411</v>
-      </c>
-      <c r="F75" t="s">
-        <v>412</v>
       </c>
       <c r="G75">
         <v>150</v>
       </c>
       <c r="H75" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I75">
         <v>1.06</v>
@@ -8265,7 +8266,7 @@
         <v>14604</v>
       </c>
       <c r="X75" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y75">
         <v>3</v>
@@ -8273,28 +8274,28 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>413</v>
+      </c>
+      <c r="B76" t="s">
         <v>414</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>415</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>416</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>417</v>
       </c>
-      <c r="E76" t="s">
-        <v>418</v>
-      </c>
       <c r="F76" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G76">
         <v>150</v>
       </c>
       <c r="H76" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I76">
         <v>1.4</v>
@@ -8339,10 +8340,10 @@
         <v>0</v>
       </c>
       <c r="W76" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="X76" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Y76">
         <v>3</v>
@@ -8350,19 +8351,19 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>419</v>
+      </c>
+      <c r="B77" t="s">
         <v>420</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>421</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>422</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>423</v>
-      </c>
-      <c r="E77" t="s">
-        <v>424</v>
       </c>
       <c r="F77" t="s">
         <v>141</v>
@@ -8371,7 +8372,7 @@
         <v>200</v>
       </c>
       <c r="H77" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I77">
         <v>1.4</v>
@@ -8419,7 +8420,7 @@
         <v>14604</v>
       </c>
       <c r="X77" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Y77">
         <v>3</v>
@@ -8427,28 +8428,28 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>424</v>
+      </c>
+      <c r="B78" t="s">
         <v>425</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>426</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>427</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>428</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>429</v>
-      </c>
-      <c r="F78" t="s">
-        <v>430</v>
       </c>
       <c r="G78">
         <v>150</v>
       </c>
       <c r="H78" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I78">
         <v>1.4</v>
@@ -8493,10 +8494,10 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="X78" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Y78">
         <v>3</v>
@@ -8504,28 +8505,28 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>433</v>
+      </c>
+      <c r="B79" t="s">
         <v>434</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>435</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>436</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>437</v>
       </c>
-      <c r="E79" t="s">
-        <v>438</v>
-      </c>
       <c r="F79" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G79">
         <v>114</v>
       </c>
       <c r="H79" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I79">
         <v>2.5299999999999998</v>
@@ -8570,10 +8571,10 @@
         <v>0</v>
       </c>
       <c r="W79" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="X79" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Y79">
         <v>3</v>
@@ -8581,19 +8582,19 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>441</v>
+      </c>
+      <c r="B80" t="s">
         <v>442</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>443</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>444</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>445</v>
-      </c>
-      <c r="E80" t="s">
-        <v>446</v>
       </c>
       <c r="F80" t="s">
         <v>134</v>
@@ -8602,7 +8603,7 @@
         <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I80">
         <v>0.67</v>
@@ -8650,7 +8651,7 @@
         <v>14193</v>
       </c>
       <c r="X80" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Y80">
         <v>3</v>
@@ -8658,19 +8659,19 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>447</v>
+      </c>
+      <c r="B81" t="s">
         <v>448</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>449</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>450</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>451</v>
-      </c>
-      <c r="E81" t="s">
-        <v>452</v>
       </c>
       <c r="F81" t="s">
         <v>134</v>
@@ -8679,7 +8680,7 @@
         <v>160</v>
       </c>
       <c r="H81" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I81">
         <v>1.4</v>
@@ -8724,10 +8725,10 @@
         <v>0</v>
       </c>
       <c r="W81" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="X81" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Y81">
         <v>3</v>
@@ -8735,19 +8736,19 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>455</v>
+      </c>
+      <c r="B82" t="s">
+        <v>454</v>
+      </c>
+      <c r="C82" t="s">
+        <v>463</v>
+      </c>
+      <c r="D82" t="s">
         <v>456</v>
       </c>
-      <c r="B82" t="s">
-        <v>455</v>
-      </c>
-      <c r="C82" t="s">
-        <v>464</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>457</v>
-      </c>
-      <c r="E82" t="s">
-        <v>458</v>
       </c>
       <c r="F82" t="s">
         <v>134</v>
@@ -8756,7 +8757,7 @@
         <v>160</v>
       </c>
       <c r="H82" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I82">
         <v>1.62</v>
@@ -8804,10 +8805,10 @@
         <v>11616</v>
       </c>
       <c r="X82" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="Y82" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the SF region to Eps Cha for 2MASS...5548 (from Charles' analysis of Gaia data)
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE9F41D-5F07-7A45-9EBD-8869C6F42E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D46D54-2116-4348-907B-A8BD810FC6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="460" windowWidth="17880" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2711,9 +2711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="108" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="108" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E73" sqref="E73"/>
+      <selection pane="topRight" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5615,7 +5615,7 @@
         <v>208</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>256</v>
       </c>
       <c r="G39">
         <v>160</v>

</xml_diff>

<commit_message>
added a few more AR targets in Taurus
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D46D54-2116-4348-907B-A8BD810FC6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FACEF5-6FA6-2540-B95B-467B2E8538F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="460" windowWidth="17880" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="505">
   <si>
     <t>2MASS</t>
   </si>
@@ -1234,9 +1234,6 @@
     <t>-78d59m34.02s</t>
   </si>
   <si>
-    <t>COS/G130M/G160M, STIS/E230M/G230L/G430L</t>
-  </si>
-  <si>
     <t>AR MODES</t>
   </si>
   <si>
@@ -1312,15 +1309,6 @@
     <t xml:space="preserve">Lupus I  </t>
   </si>
   <si>
-    <t>COS/G130M/G140L/G160M, STIS/G230L/G430L</t>
-  </si>
-  <si>
-    <t>COS/G130M/G140L/G160M, STIS/G140L/G230L/G230MB/G430L</t>
-  </si>
-  <si>
-    <t>COS/G130M/G140L/G160M, STIS/G230L/G230M/G430L</t>
-  </si>
-  <si>
     <t>HD 104237A</t>
   </si>
   <si>
@@ -1381,9 +1369,6 @@
     <t xml:space="preserve">K2 </t>
   </si>
   <si>
-    <t>COS/G130M/G160M, STIS/E230M/G140L/G230L/G430L/G750L</t>
-  </si>
-  <si>
     <t>J11122772-7644223</t>
   </si>
   <si>
@@ -1414,9 +1399,6 @@
     <t>T52</t>
   </si>
   <si>
-    <t>3Check</t>
-  </si>
-  <si>
     <t>11616|12876|</t>
   </si>
   <si>
@@ -1445,13 +1427,121 @@
   </si>
   <si>
     <t>-78d54m42.74s</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M-STIS/E230M/G230L/G430L</t>
+  </si>
+  <si>
+    <t>COS/G130M/G140L/G160M-STIS/G230L/G430L</t>
+  </si>
+  <si>
+    <t>COS/G130M/G140L/G160M- STIS/G140L/G230L/G230MB/G430L</t>
+  </si>
+  <si>
+    <t>COS/G130M/G140L/G160M- STIS/G230L/G230M/G430L</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M-STIS/E230M/G140L/G230L/G430L/G750L</t>
+  </si>
+  <si>
+    <t>LkCa 15</t>
+  </si>
+  <si>
+    <t>J04391779+2221034</t>
+  </si>
+  <si>
+    <t>V1079 Tau</t>
+  </si>
+  <si>
+    <t>4h39m17.73s</t>
+  </si>
+  <si>
+    <t>+22d21m03.8s</t>
+  </si>
+  <si>
+    <t>9374|11616|14698</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M-STIS/G140L/G230L/G430L/G750M/E230M</t>
+  </si>
+  <si>
+    <t>LkCa 19</t>
+  </si>
+  <si>
+    <t>J04553695+3017553</t>
+  </si>
+  <si>
+    <t>HD282630</t>
+  </si>
+  <si>
+    <t>4h55m36.97s</t>
+  </si>
+  <si>
+    <t>+30d17m55.0s</t>
+  </si>
+  <si>
+    <t>11608|11616</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M-STIS/G230L/G430L/G750L/E230M</t>
+  </si>
+  <si>
+    <t>LkCa 4</t>
+  </si>
+  <si>
+    <t>J04162810+2807358</t>
+  </si>
+  <si>
+    <t>4h16m28.11s</t>
+  </si>
+  <si>
+    <t>+28d07m35.73s</t>
+  </si>
+  <si>
+    <t>9790|11616</t>
+  </si>
+  <si>
+    <t>AA Tau</t>
+  </si>
+  <si>
+    <t>J04345542+2428531</t>
+  </si>
+  <si>
+    <t>HBC 63</t>
+  </si>
+  <si>
+    <t>4h34m55.42s</t>
+  </si>
+  <si>
+    <t>+24d28m52.8s</t>
+  </si>
+  <si>
+    <t>11616|12876|15070</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M-STIS/E230M/G230L/G430L/G230M</t>
+  </si>
+  <si>
+    <t>DE Tau</t>
+  </si>
+  <si>
+    <t>J04215563+2755060</t>
+  </si>
+  <si>
+    <t>4h21m55.69s</t>
+  </si>
+  <si>
+    <t>+27d55m06.1s</t>
+  </si>
+  <si>
+    <t>8628|11616</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1589,6 +1679,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF010101"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1935,7 +2032,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
@@ -1943,6 +2040,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1988,7 +2086,187 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="59">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2709,11 +2987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y82"/>
+  <dimension ref="A1:Y87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA85" sqref="AA85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2724,12 +3002,12 @@
     <col min="16" max="17" width="12.5" customWidth="1"/>
     <col min="18" max="18" width="14.5" customWidth="1"/>
     <col min="19" max="19" width="18.33203125" customWidth="1"/>
-    <col min="24" max="24" width="15.5" customWidth="1"/>
+    <col min="24" max="24" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2786,22 +3064,22 @@
         <v>13</v>
       </c>
       <c r="T1" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="U1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="V1" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="W1" t="s">
         <v>363</v>
       </c>
       <c r="X1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="Y1" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2879,7 +3157,7 @@
         <v>16115</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -3738,7 +4016,7 @@
         <v>16114</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="Y13">
         <v>2</v>
@@ -5885,7 +6163,7 @@
         <v>16482</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
@@ -7913,7 +8191,7 @@
         <v>361</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="F71" t="s">
         <v>362</v>
@@ -8032,10 +8310,10 @@
         <v>0</v>
       </c>
       <c r="W72" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="X72" t="s">
-        <v>404</v>
+        <v>469</v>
       </c>
       <c r="Y72">
         <v>3</v>
@@ -8112,7 +8390,7 @@
         <v>11616</v>
       </c>
       <c r="X73" t="s">
-        <v>404</v>
+        <v>469</v>
       </c>
       <c r="Y73">
         <v>3</v>
@@ -8189,7 +8467,7 @@
         <v>11616</v>
       </c>
       <c r="X74" t="s">
-        <v>404</v>
+        <v>469</v>
       </c>
       <c r="Y74">
         <v>3</v>
@@ -8197,28 +8475,28 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>405</v>
+      </c>
+      <c r="B75" t="s">
         <v>406</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>407</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>408</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>409</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F75" t="s">
         <v>410</v>
-      </c>
-      <c r="F75" t="s">
-        <v>411</v>
       </c>
       <c r="G75">
         <v>150</v>
       </c>
       <c r="H75" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I75">
         <v>1.06</v>
@@ -8266,7 +8544,7 @@
         <v>14604</v>
       </c>
       <c r="X75" t="s">
-        <v>430</v>
+        <v>470</v>
       </c>
       <c r="Y75">
         <v>3</v>
@@ -8274,28 +8552,28 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>412</v>
+      </c>
+      <c r="B76" t="s">
         <v>413</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>414</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>415</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>416</v>
       </c>
-      <c r="E76" t="s">
-        <v>417</v>
-      </c>
       <c r="F76" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G76">
         <v>150</v>
       </c>
       <c r="H76" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I76">
         <v>1.4</v>
@@ -8340,10 +8618,10 @@
         <v>0</v>
       </c>
       <c r="W76" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="X76" t="s">
-        <v>431</v>
+        <v>471</v>
       </c>
       <c r="Y76">
         <v>3</v>
@@ -8351,19 +8629,19 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>418</v>
+      </c>
+      <c r="B77" t="s">
         <v>419</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>420</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>421</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>422</v>
-      </c>
-      <c r="E77" t="s">
-        <v>423</v>
       </c>
       <c r="F77" t="s">
         <v>141</v>
@@ -8372,7 +8650,7 @@
         <v>200</v>
       </c>
       <c r="H77" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I77">
         <v>1.4</v>
@@ -8420,7 +8698,7 @@
         <v>14604</v>
       </c>
       <c r="X77" t="s">
-        <v>430</v>
+        <v>470</v>
       </c>
       <c r="Y77">
         <v>3</v>
@@ -8428,28 +8706,28 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>423</v>
+      </c>
+      <c r="B78" t="s">
         <v>424</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>425</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>426</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>427</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>428</v>
-      </c>
-      <c r="F78" t="s">
-        <v>429</v>
       </c>
       <c r="G78">
         <v>150</v>
       </c>
       <c r="H78" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I78">
         <v>1.4</v>
@@ -8494,10 +8772,10 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="X78" t="s">
-        <v>432</v>
+        <v>472</v>
       </c>
       <c r="Y78">
         <v>3</v>
@@ -8505,28 +8783,28 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>429</v>
+      </c>
+      <c r="B79" t="s">
+        <v>430</v>
+      </c>
+      <c r="C79" t="s">
+        <v>431</v>
+      </c>
+      <c r="D79" t="s">
+        <v>432</v>
+      </c>
+      <c r="E79" t="s">
         <v>433</v>
       </c>
-      <c r="B79" t="s">
-        <v>434</v>
-      </c>
-      <c r="C79" t="s">
-        <v>435</v>
-      </c>
-      <c r="D79" t="s">
-        <v>436</v>
-      </c>
-      <c r="E79" t="s">
-        <v>437</v>
-      </c>
       <c r="F79" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="G79">
         <v>114</v>
       </c>
       <c r="H79" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="I79">
         <v>2.5299999999999998</v>
@@ -8571,10 +8849,10 @@
         <v>0</v>
       </c>
       <c r="W79" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="X79" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="Y79">
         <v>3</v>
@@ -8582,19 +8860,19 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>437</v>
+      </c>
+      <c r="B80" t="s">
+        <v>438</v>
+      </c>
+      <c r="C80" t="s">
+        <v>439</v>
+      </c>
+      <c r="D80" t="s">
+        <v>440</v>
+      </c>
+      <c r="E80" t="s">
         <v>441</v>
-      </c>
-      <c r="B80" t="s">
-        <v>442</v>
-      </c>
-      <c r="C80" t="s">
-        <v>443</v>
-      </c>
-      <c r="D80" t="s">
-        <v>444</v>
-      </c>
-      <c r="E80" t="s">
-        <v>445</v>
       </c>
       <c r="F80" t="s">
         <v>134</v>
@@ -8603,7 +8881,7 @@
         <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="I80">
         <v>0.67</v>
@@ -8651,7 +8929,7 @@
         <v>14193</v>
       </c>
       <c r="X80" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="Y80">
         <v>3</v>
@@ -8659,19 +8937,19 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>443</v>
+      </c>
+      <c r="B81" t="s">
+        <v>444</v>
+      </c>
+      <c r="C81" t="s">
+        <v>445</v>
+      </c>
+      <c r="D81" t="s">
+        <v>446</v>
+      </c>
+      <c r="E81" t="s">
         <v>447</v>
-      </c>
-      <c r="B81" t="s">
-        <v>448</v>
-      </c>
-      <c r="C81" t="s">
-        <v>449</v>
-      </c>
-      <c r="D81" t="s">
-        <v>450</v>
-      </c>
-      <c r="E81" t="s">
-        <v>451</v>
       </c>
       <c r="F81" t="s">
         <v>134</v>
@@ -8680,7 +8958,7 @@
         <v>160</v>
       </c>
       <c r="H81" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="I81">
         <v>1.4</v>
@@ -8725,10 +9003,10 @@
         <v>0</v>
       </c>
       <c r="W81" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="X81" t="s">
-        <v>453</v>
+        <v>473</v>
       </c>
       <c r="Y81">
         <v>3</v>
@@ -8736,19 +9014,19 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B82" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C82" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D82" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E82" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="F82" t="s">
         <v>134</v>
@@ -8757,7 +9035,7 @@
         <v>160</v>
       </c>
       <c r="H82" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="I82">
         <v>1.62</v>
@@ -8805,188 +9083,630 @@
         <v>11616</v>
       </c>
       <c r="X82" t="s">
-        <v>459</v>
-      </c>
-      <c r="Y82" t="s">
-        <v>464</v>
+        <v>454</v>
+      </c>
+      <c r="Y82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>474</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="C83" t="s">
+        <v>476</v>
+      </c>
+      <c r="D83" t="s">
+        <v>477</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="F83" t="s">
+        <v>360</v>
+      </c>
+      <c r="G83">
+        <v>140</v>
+      </c>
+      <c r="H83" t="s">
+        <v>293</v>
+      </c>
+      <c r="I83">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J83">
+        <v>-8.51</v>
+      </c>
+      <c r="K83">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M83">
+        <v>12.03</v>
+      </c>
+      <c r="N83">
+        <v>2</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>0</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+      <c r="S83">
+        <v>0</v>
+      </c>
+      <c r="T83">
+        <v>0</v>
+      </c>
+      <c r="U83">
+        <v>0</v>
+      </c>
+      <c r="V83">
+        <v>0</v>
+      </c>
+      <c r="W83" t="s">
+        <v>479</v>
+      </c>
+      <c r="X83" t="s">
+        <v>480</v>
+      </c>
+      <c r="Y83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>481</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C84" t="s">
+        <v>483</v>
+      </c>
+      <c r="D84" t="s">
+        <v>484</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="F84" t="s">
+        <v>360</v>
+      </c>
+      <c r="G84">
+        <v>140</v>
+      </c>
+      <c r="H84" t="s">
+        <v>251</v>
+      </c>
+      <c r="I84">
+        <v>1.3</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>11.12</v>
+      </c>
+      <c r="N84">
+        <v>2</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>0</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+      <c r="S84">
+        <v>0</v>
+      </c>
+      <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <v>0</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84" t="s">
+        <v>486</v>
+      </c>
+      <c r="X84" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>488</v>
+      </c>
+      <c r="B85" t="s">
+        <v>489</v>
+      </c>
+      <c r="D85" t="s">
+        <v>490</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="F85" t="s">
+        <v>360</v>
+      </c>
+      <c r="G85">
+        <v>140</v>
+      </c>
+      <c r="H85" t="s">
+        <v>25</v>
+      </c>
+      <c r="I85">
+        <v>0.77</v>
+      </c>
+      <c r="K85">
+        <v>0.69</v>
+      </c>
+      <c r="M85">
+        <v>12.78</v>
+      </c>
+      <c r="N85">
+        <v>2</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85">
+        <v>0</v>
+      </c>
+      <c r="T85">
+        <v>0</v>
+      </c>
+      <c r="U85">
+        <v>0</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+      <c r="W85" t="s">
+        <v>492</v>
+      </c>
+      <c r="X85" t="s">
+        <v>469</v>
+      </c>
+      <c r="Y85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>493</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="C86" t="s">
+        <v>495</v>
+      </c>
+      <c r="D86" t="s">
+        <v>496</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="F86" t="s">
+        <v>360</v>
+      </c>
+      <c r="G86">
+        <v>140</v>
+      </c>
+      <c r="H86" t="s">
+        <v>25</v>
+      </c>
+      <c r="I86">
+        <v>0.8</v>
+      </c>
+      <c r="J86">
+        <v>-7.82</v>
+      </c>
+      <c r="K86">
+        <v>1.9</v>
+      </c>
+      <c r="L86">
+        <v>13.14</v>
+      </c>
+      <c r="M86">
+        <v>12.2</v>
+      </c>
+      <c r="N86">
+        <v>2</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="Q86">
+        <v>0</v>
+      </c>
+      <c r="R86">
+        <v>0</v>
+      </c>
+      <c r="S86">
+        <v>0</v>
+      </c>
+      <c r="T86">
+        <v>0</v>
+      </c>
+      <c r="U86">
+        <v>0</v>
+      </c>
+      <c r="V86">
+        <v>0</v>
+      </c>
+      <c r="W86" t="s">
+        <v>498</v>
+      </c>
+      <c r="X86" t="s">
+        <v>499</v>
+      </c>
+      <c r="Y86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>500</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="D87" t="s">
+        <v>502</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="F87" t="s">
+        <v>360</v>
+      </c>
+      <c r="G87">
+        <v>140</v>
+      </c>
+      <c r="H87" t="s">
+        <v>100</v>
+      </c>
+      <c r="I87">
+        <v>0.4</v>
+      </c>
+      <c r="J87">
+        <v>-7.55</v>
+      </c>
+      <c r="K87">
+        <v>0.9</v>
+      </c>
+      <c r="L87">
+        <v>15.18</v>
+      </c>
+      <c r="M87">
+        <v>13.8</v>
+      </c>
+      <c r="N87">
+        <v>2</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+      <c r="R87">
+        <v>0</v>
+      </c>
+      <c r="S87">
+        <v>0</v>
+      </c>
+      <c r="T87">
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <v>0</v>
+      </c>
+      <c r="V87">
+        <v>0</v>
+      </c>
+      <c r="W87" t="s">
+        <v>504</v>
+      </c>
+      <c r="X87" t="s">
+        <v>499</v>
+      </c>
+      <c r="Y87">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="40" priority="38">
+    <cfRule type="expression" dxfId="58" priority="56">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="41">
+    <cfRule type="expression" dxfId="57" priority="59">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72">
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="56" priority="55">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="40">
+    <cfRule type="expression" dxfId="55" priority="58">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72">
-    <cfRule type="expression" dxfId="36" priority="39">
+    <cfRule type="expression" dxfId="54" priority="57">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="53" priority="54">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="52" priority="53">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="50" priority="49">
+      <formula>$N73=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="49" priority="51">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="48" priority="50">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W74 Y74">
+    <cfRule type="expression" dxfId="47" priority="46">
+      <formula>$N74=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="48">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W74 Y74">
+    <cfRule type="expression" dxfId="45" priority="47">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+    <cfRule type="expression" dxfId="44" priority="43">
+      <formula>$N75=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+    <cfRule type="expression" dxfId="42" priority="44">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N79">
+    <cfRule type="expression" dxfId="41" priority="40">
+      <formula>$N79=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="42">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N79">
+    <cfRule type="expression" dxfId="39" priority="41">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O79:W79">
+    <cfRule type="expression" dxfId="38" priority="37">
+      <formula>$N79=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="39">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O79:W79">
+    <cfRule type="expression" dxfId="36" priority="38">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N80">
+    <cfRule type="expression" dxfId="35" priority="34">
+      <formula>$N80=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="36">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N80">
+    <cfRule type="expression" dxfId="33" priority="35">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="32" priority="31">
-      <formula>$N73=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="31" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="29" priority="28">
-      <formula>$N74=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="27" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="26" priority="25">
-      <formula>$N75=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="24" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N82">
     <cfRule type="expression" dxfId="23" priority="22">
-      <formula>$N79=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N82">
     <cfRule type="expression" dxfId="21" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O82:W82">
     <cfRule type="expression" dxfId="20" priority="19">
-      <formula>$N79=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O82:W82">
     <cfRule type="expression" dxfId="18" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="Y83:Y87">
     <cfRule type="expression" dxfId="17" priority="16">
-      <formula>$N80=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="Y83:Y87">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="14" priority="13">
-      <formula>$N80=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="11" priority="10">
-      <formula>$N81=0</formula>
+      <formula>$N84=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="8" priority="7">
-      <formula>$N81=0</formula>
+      <formula>$N85=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="6" priority="8">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N82=0</formula>
+      <formula>$N86=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
+  <conditionalFormatting sqref="O87:V87">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N82=0</formula>
+      <formula>$N87=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
+  <conditionalFormatting sqref="O87:V87">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added a few more archival CTTS
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FACEF5-6FA6-2540-B95B-467B2E8538F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2CD063-FD3B-9442-92BD-6498CDE84FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="460" windowWidth="17880" windowHeight="19060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8120" yWindow="460" windowWidth="29640" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="526">
   <si>
     <t>2MASS</t>
   </si>
@@ -1535,6 +1535,69 @@
   </si>
   <si>
     <t>8628|11616</t>
+  </si>
+  <si>
+    <t>4h30m44.25s</t>
+  </si>
+  <si>
+    <t>+26d01m24.5s</t>
+  </si>
+  <si>
+    <t>DK Tau A</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M-STIS/G230L/G430L/E230M</t>
+  </si>
+  <si>
+    <t>DM Tau</t>
+  </si>
+  <si>
+    <t>9374|11608|11616</t>
+  </si>
+  <si>
+    <t>J04334871+1810099</t>
+  </si>
+  <si>
+    <t>HBC 62</t>
+  </si>
+  <si>
+    <t>4h33m48.74s</t>
+  </si>
+  <si>
+    <t>+18d10m09.7s</t>
+  </si>
+  <si>
+    <t>DN Tau</t>
+  </si>
+  <si>
+    <t>4h35m27.44s</t>
+  </si>
+  <si>
+    <t>+24d14m59.1s</t>
+  </si>
+  <si>
+    <t>DR Tau</t>
+  </si>
+  <si>
+    <t>4h47m06.22s+16d58m42.6s</t>
+  </si>
+  <si>
+    <t>J04470620+1658428</t>
+  </si>
+  <si>
+    <t>HBC 74</t>
+  </si>
+  <si>
+    <t>J04352737+2414589</t>
+  </si>
+  <si>
+    <t>HBC 65</t>
+  </si>
+  <si>
+    <t>8206|8627|11616</t>
+  </si>
+  <si>
+    <t>COS/G130M/G160M</t>
   </si>
 </sst>
 </file>
@@ -2086,7 +2149,127 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="71">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2987,11 +3170,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y87"/>
+  <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA85" sqref="AA85"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z96" sqref="Z96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9453,260 +9636,605 @@
         <v>3</v>
       </c>
     </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>507</v>
+      </c>
+      <c r="D88" t="s">
+        <v>505</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="F88" t="s">
+        <v>360</v>
+      </c>
+      <c r="G88">
+        <v>140</v>
+      </c>
+      <c r="H88" t="s">
+        <v>25</v>
+      </c>
+      <c r="I88">
+        <v>0.7</v>
+      </c>
+      <c r="J88">
+        <v>-7.47</v>
+      </c>
+      <c r="K88">
+        <v>1.3</v>
+      </c>
+      <c r="N88">
+        <v>2</v>
+      </c>
+      <c r="O88">
+        <v>0</v>
+      </c>
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88">
+        <v>0</v>
+      </c>
+      <c r="R88">
+        <v>0</v>
+      </c>
+      <c r="S88">
+        <v>0</v>
+      </c>
+      <c r="T88">
+        <v>0</v>
+      </c>
+      <c r="U88">
+        <v>0</v>
+      </c>
+      <c r="V88">
+        <v>0</v>
+      </c>
+      <c r="W88">
+        <v>11616</v>
+      </c>
+      <c r="X88" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>509</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="C89" t="s">
+        <v>512</v>
+      </c>
+      <c r="D89" t="s">
+        <v>513</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="F89" t="s">
+        <v>360</v>
+      </c>
+      <c r="G89">
+        <v>140</v>
+      </c>
+      <c r="H89" t="s">
+        <v>142</v>
+      </c>
+      <c r="I89">
+        <v>0.5</v>
+      </c>
+      <c r="J89">
+        <v>-8.5399999999999991</v>
+      </c>
+      <c r="K89">
+        <v>0.7</v>
+      </c>
+      <c r="L89">
+        <v>14.3</v>
+      </c>
+      <c r="M89">
+        <v>14</v>
+      </c>
+      <c r="N89">
+        <v>2</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>0</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+      <c r="S89">
+        <v>0</v>
+      </c>
+      <c r="T89">
+        <v>0</v>
+      </c>
+      <c r="U89">
+        <v>0</v>
+      </c>
+      <c r="V89">
+        <v>0</v>
+      </c>
+      <c r="W89" t="s">
+        <v>510</v>
+      </c>
+      <c r="X89" t="s">
+        <v>473</v>
+      </c>
+      <c r="Y89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>515</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C90" t="s">
+        <v>523</v>
+      </c>
+      <c r="D90" t="s">
+        <v>516</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="F90" t="s">
+        <v>360</v>
+      </c>
+      <c r="G90">
+        <v>140</v>
+      </c>
+      <c r="H90" t="s">
+        <v>20</v>
+      </c>
+      <c r="I90">
+        <v>0.6</v>
+      </c>
+      <c r="J90">
+        <v>-8</v>
+      </c>
+      <c r="K90">
+        <v>0.9</v>
+      </c>
+      <c r="L90">
+        <v>13.56</v>
+      </c>
+      <c r="M90">
+        <v>11.5</v>
+      </c>
+      <c r="N90">
+        <v>2</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+      <c r="S90">
+        <v>0</v>
+      </c>
+      <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="U90">
+        <v>0</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>11616</v>
+      </c>
+      <c r="X90" t="s">
+        <v>508</v>
+      </c>
+      <c r="Y90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>518</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="C91" t="s">
+        <v>521</v>
+      </c>
+      <c r="D91" t="s">
+        <v>519</v>
+      </c>
+      <c r="F91" t="s">
+        <v>360</v>
+      </c>
+      <c r="G91">
+        <v>140</v>
+      </c>
+      <c r="H91" t="s">
+        <v>293</v>
+      </c>
+      <c r="I91">
+        <v>0.9</v>
+      </c>
+      <c r="J91">
+        <v>-7.28</v>
+      </c>
+      <c r="K91">
+        <v>1.4</v>
+      </c>
+      <c r="L91">
+        <v>12.03</v>
+      </c>
+      <c r="M91">
+        <v>10.5</v>
+      </c>
+      <c r="N91">
+        <v>2</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="R91">
+        <v>0</v>
+      </c>
+      <c r="S91">
+        <v>0</v>
+      </c>
+      <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="U91">
+        <v>0</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+      <c r="W91" t="s">
+        <v>524</v>
+      </c>
+      <c r="X91" t="s">
+        <v>525</v>
+      </c>
+      <c r="Y91">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A16:X33">
-    <cfRule type="expression" dxfId="58" priority="56">
+    <cfRule type="expression" dxfId="70" priority="68">
       <formula>$N16=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="59">
+    <cfRule type="expression" dxfId="69" priority="71">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72">
-    <cfRule type="expression" dxfId="56" priority="55">
+    <cfRule type="expression" dxfId="68" priority="67">
       <formula>$N39=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="58">
+    <cfRule type="expression" dxfId="67" priority="70">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72">
-    <cfRule type="expression" dxfId="54" priority="57">
+    <cfRule type="expression" dxfId="66" priority="69">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="expression" dxfId="53" priority="54">
+    <cfRule type="expression" dxfId="65" priority="66">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="expression" dxfId="52" priority="53">
+    <cfRule type="expression" dxfId="64" priority="65">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70">
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="63" priority="64">
       <formula>$E70=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="62" priority="61">
+      <formula>$N73=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="63">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O73:W73 Y73">
+    <cfRule type="expression" dxfId="60" priority="62">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W74 Y74">
+    <cfRule type="expression" dxfId="59" priority="58">
+      <formula>$N74=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="60">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O74:W74 Y74">
+    <cfRule type="expression" dxfId="57" priority="59">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+    <cfRule type="expression" dxfId="56" priority="55">
+      <formula>$N75=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="57">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+    <cfRule type="expression" dxfId="54" priority="56">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N79">
+    <cfRule type="expression" dxfId="53" priority="52">
+      <formula>$N79=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="54">
+      <formula>"$N2=0"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N79">
+    <cfRule type="expression" dxfId="51" priority="53">
+      <formula>$N$2=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O79:W79">
     <cfRule type="expression" dxfId="50" priority="49">
-      <formula>$N73=0</formula>
+      <formula>$N79=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="49" priority="51">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O73:W73 Y73">
+  <conditionalFormatting sqref="O79:W79">
     <cfRule type="expression" dxfId="48" priority="50">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
+  <conditionalFormatting sqref="N80">
     <cfRule type="expression" dxfId="47" priority="46">
-      <formula>$N74=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="46" priority="48">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O74:W74 Y74">
+  <conditionalFormatting sqref="N80">
     <cfRule type="expression" dxfId="45" priority="47">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="44" priority="43">
-      <formula>$N75=0</formula>
+      <formula>$N80=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="43" priority="45">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O75:W78 Y75:Y81">
+  <conditionalFormatting sqref="O80:W80">
     <cfRule type="expression" dxfId="42" priority="44">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="41" priority="40">
-      <formula>$N79=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="40" priority="42">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N79">
+  <conditionalFormatting sqref="N81">
     <cfRule type="expression" dxfId="39" priority="41">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="38" priority="37">
-      <formula>$N79=0</formula>
+      <formula>$N81=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="37" priority="39">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O79:W79">
+  <conditionalFormatting sqref="O81:W81">
     <cfRule type="expression" dxfId="36" priority="38">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="N82">
     <cfRule type="expression" dxfId="35" priority="34">
-      <formula>$N80=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="34" priority="36">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N80">
+  <conditionalFormatting sqref="N82">
     <cfRule type="expression" dxfId="33" priority="35">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O82:W82">
     <cfRule type="expression" dxfId="32" priority="31">
-      <formula>$N80=0</formula>
+      <formula>$N82=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="31" priority="33">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O80:W80">
+  <conditionalFormatting sqref="O82:W82">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="Y83:Y91">
     <cfRule type="expression" dxfId="29" priority="28">
-      <formula>$N81=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N81">
+  <conditionalFormatting sqref="Y83:Y91">
     <cfRule type="expression" dxfId="27" priority="29">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="26" priority="25">
-      <formula>$N81=0</formula>
+      <formula>$N83=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="25" priority="27">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O81:W81">
+  <conditionalFormatting sqref="O83:V83">
     <cfRule type="expression" dxfId="24" priority="26">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="23" priority="22">
-      <formula>$N82=0</formula>
+      <formula>$N84=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="22" priority="24">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N82">
+  <conditionalFormatting sqref="O84:V84">
     <cfRule type="expression" dxfId="21" priority="23">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="20" priority="19">
-      <formula>$N82=0</formula>
+      <formula>$N85=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="19" priority="21">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O82:W82">
+  <conditionalFormatting sqref="O85:V85">
     <cfRule type="expression" dxfId="18" priority="20">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y87">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="17" priority="16">
-      <formula>$N83=0</formula>
+      <formula>$N86=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y83:Y87">
+  <conditionalFormatting sqref="O86:V86">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O87:V87">
     <cfRule type="expression" dxfId="14" priority="13">
-      <formula>$N83=0</formula>
+      <formula>$N87=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O83:V83">
+  <conditionalFormatting sqref="O87:V87">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O88:W88 W89">
     <cfRule type="expression" dxfId="11" priority="10">
-      <formula>$N84=0</formula>
+      <formula>$N88=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O84:V84">
+  <conditionalFormatting sqref="O88:W88 W89">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O89:V89">
     <cfRule type="expression" dxfId="8" priority="7">
-      <formula>$N85=0</formula>
+      <formula>$N89=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O85:V85">
+  <conditionalFormatting sqref="O89:V89">
     <cfRule type="expression" dxfId="6" priority="8">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O90:W90 W91">
     <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$N86=0</formula>
+      <formula>$N90=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O86:V86">
+  <conditionalFormatting sqref="O90:W90 W91">
     <cfRule type="expression" dxfId="3" priority="5">
       <formula>$N$2=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
+  <conditionalFormatting sqref="O91:V91">
     <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$N87=0</formula>
+      <formula>$N91=0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O87:V87">
+  <conditionalFormatting sqref="O91:V91">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fixed upper case of Eta Cha and Eps cha
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2CD063-FD3B-9442-92BD-6498CDE84FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7B2F1-79E5-8A4C-B93D-0FAAEF330A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8120" yWindow="460" windowWidth="29640" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="524">
   <si>
     <t>2MASS</t>
   </si>
@@ -577,9 +577,6 @@
     <t>-78d57m44.48s</t>
   </si>
   <si>
-    <t>eta Cha</t>
-  </si>
-  <si>
     <t>J08441637-7859080</t>
   </si>
   <si>
@@ -788,9 +785,6 @@
   </si>
   <si>
     <t>-78d11m42.2s</t>
-  </si>
-  <si>
-    <t>eps Cha</t>
   </si>
   <si>
     <t>J11083952-7734166</t>
@@ -3172,9 +3166,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z96" sqref="Z96"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3190,7 +3184,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3229,16 +3223,16 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="P1" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q1" t="s">
         <v>355</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>357</v>
       </c>
       <c r="R1" t="s">
         <v>12</v>
@@ -3247,22 +3241,22 @@
         <v>13</v>
       </c>
       <c r="T1" t="s">
+        <v>463</v>
+      </c>
+      <c r="U1" t="s">
+        <v>464</v>
+      </c>
+      <c r="V1" t="s">
         <v>465</v>
       </c>
-      <c r="U1" t="s">
-        <v>466</v>
-      </c>
-      <c r="V1" t="s">
-        <v>467</v>
-      </c>
       <c r="W1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="X1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="Y1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3340,7 +3334,7 @@
         <v>16115</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -3504,7 +3498,7 @@
     </row>
     <row r="5" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -3583,7 +3577,7 @@
     </row>
     <row r="6" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>38</v>
@@ -3816,7 +3810,7 @@
     </row>
     <row r="9" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>53</v>
@@ -4199,7 +4193,7 @@
         <v>16114</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Y13">
         <v>2</v>
@@ -4284,7 +4278,7 @@
     </row>
     <row r="15" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>79</v>
@@ -5184,7 +5178,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>149</v>
@@ -5332,7 +5326,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B29" t="s">
         <v>158</v>
@@ -5480,7 +5474,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B31" t="s">
         <v>167</v>
@@ -5693,7 +5687,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>181</v>
@@ -5708,7 +5702,7 @@
         <v>184</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="G34" s="3">
         <v>94</v>
@@ -5765,22 +5759,22 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="G35" s="3">
         <v>94</v>
@@ -5837,28 +5831,28 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>193</v>
-      </c>
       <c r="F36" s="6" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="G36" s="6">
         <v>94</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I36" s="6">
         <v>5.1999999999999998E-2</v>
@@ -5913,22 +5907,22 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="G37" s="2">
         <v>94</v>
@@ -5987,28 +5981,28 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>185</v>
+        <v>360</v>
       </c>
       <c r="G38" s="2">
         <v>94</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I38" s="2">
         <v>0.28999999999999998</v>
@@ -6061,22 +6055,22 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" t="s">
         <v>204</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>205</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>206</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>207</v>
       </c>
-      <c r="E39" t="s">
-        <v>208</v>
-      </c>
       <c r="F39" t="s">
-        <v>256</v>
+        <v>454</v>
       </c>
       <c r="G39">
         <v>160</v>
@@ -6127,19 +6121,19 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>134</v>
@@ -6148,7 +6142,7 @@
         <v>160</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I40" s="6">
         <v>0.14000000000000001</v>
@@ -6199,17 +6193,17 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>134</v>
@@ -6218,7 +6212,7 @@
         <v>160</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I41" s="6">
         <v>1.25</v>
@@ -6273,19 +6267,19 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>134</v>
@@ -6346,24 +6340,24 @@
         <v>16482</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>228</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>134</v>
@@ -6427,19 +6421,19 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C44" t="s">
         <v>229</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>230</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>231</v>
-      </c>
-      <c r="E44" t="s">
-        <v>232</v>
       </c>
       <c r="F44" t="s">
         <v>134</v>
@@ -6499,19 +6493,19 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>134</v>
@@ -6575,19 +6569,19 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B46" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" t="s">
         <v>238</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>239</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>240</v>
-      </c>
-      <c r="E46" t="s">
-        <v>241</v>
       </c>
       <c r="F46" t="s">
         <v>134</v>
@@ -6596,7 +6590,7 @@
         <v>160</v>
       </c>
       <c r="H46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I46">
         <v>1.31</v>
@@ -6647,19 +6641,19 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B47" t="s">
+        <v>241</v>
+      </c>
+      <c r="C47" t="s">
         <v>242</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>243</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>244</v>
-      </c>
-      <c r="E47" t="s">
-        <v>245</v>
       </c>
       <c r="F47" t="s">
         <v>134</v>
@@ -6719,19 +6713,19 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>245</v>
+      </c>
+      <c r="B48" t="s">
         <v>246</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>247</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>248</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>249</v>
-      </c>
-      <c r="E48" t="s">
-        <v>250</v>
       </c>
       <c r="F48" t="s">
         <v>134</v>
@@ -6740,7 +6734,7 @@
         <v>160</v>
       </c>
       <c r="H48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I48">
         <v>2.08</v>
@@ -6791,22 +6785,22 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C49" t="s">
         <v>252</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>253</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>254</v>
       </c>
-      <c r="E49" t="s">
-        <v>255</v>
-      </c>
       <c r="F49" t="s">
-        <v>256</v>
+        <v>454</v>
       </c>
       <c r="G49">
         <v>114</v>
@@ -6863,19 +6857,19 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B50" t="s">
+        <v>255</v>
+      </c>
+      <c r="C50" t="s">
+        <v>256</v>
+      </c>
+      <c r="D50" t="s">
         <v>257</v>
       </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
         <v>258</v>
-      </c>
-      <c r="D50" t="s">
-        <v>259</v>
-      </c>
-      <c r="E50" t="s">
-        <v>260</v>
       </c>
       <c r="F50" t="s">
         <v>134</v>
@@ -6884,7 +6878,7 @@
         <v>160</v>
       </c>
       <c r="H50" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I50">
         <v>0.1</v>
@@ -6935,22 +6929,22 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>260</v>
+      </c>
+      <c r="B51" t="s">
+        <v>261</v>
+      </c>
+      <c r="C51" t="s">
         <v>262</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>263</v>
       </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>264</v>
       </c>
-      <c r="D51" t="s">
-        <v>265</v>
-      </c>
-      <c r="E51" t="s">
-        <v>266</v>
-      </c>
       <c r="F51" t="s">
-        <v>256</v>
+        <v>454</v>
       </c>
       <c r="G51">
         <v>114</v>
@@ -7007,19 +7001,19 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>265</v>
+      </c>
+      <c r="B52" t="s">
+        <v>266</v>
+      </c>
+      <c r="C52" t="s">
         <v>267</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>268</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>269</v>
-      </c>
-      <c r="D52" t="s">
-        <v>270</v>
-      </c>
-      <c r="E52" t="s">
-        <v>271</v>
       </c>
       <c r="F52" t="s">
         <v>141</v>
@@ -7079,28 +7073,28 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>270</v>
+      </c>
+      <c r="B53" t="s">
+        <v>271</v>
+      </c>
+      <c r="C53" t="s">
         <v>272</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>273</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>274</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>275</v>
-      </c>
-      <c r="E53" t="s">
-        <v>276</v>
-      </c>
-      <c r="F53" t="s">
-        <v>277</v>
       </c>
       <c r="G53">
         <v>130</v>
       </c>
       <c r="H53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I53">
         <v>0.93</v>
@@ -7151,16 +7145,16 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>276</v>
+      </c>
+      <c r="B54" t="s">
+        <v>277</v>
+      </c>
+      <c r="D54" t="s">
         <v>278</v>
       </c>
-      <c r="B54" t="s">
+      <c r="E54" t="s">
         <v>279</v>
-      </c>
-      <c r="D54" t="s">
-        <v>280</v>
-      </c>
-      <c r="E54" t="s">
-        <v>281</v>
       </c>
       <c r="F54" t="s">
         <v>89</v>
@@ -7220,22 +7214,22 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>280</v>
+      </c>
+      <c r="B55" t="s">
+        <v>281</v>
+      </c>
+      <c r="C55" t="s">
         <v>282</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>283</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
         <v>284</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
         <v>285</v>
-      </c>
-      <c r="E55" t="s">
-        <v>286</v>
-      </c>
-      <c r="F55" t="s">
-        <v>287</v>
       </c>
       <c r="G55">
         <v>150</v>
@@ -7292,28 +7286,28 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>286</v>
+      </c>
+      <c r="B56" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" t="s">
         <v>288</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>289</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
         <v>290</v>
       </c>
-      <c r="D56" t="s">
-        <v>291</v>
-      </c>
-      <c r="E56" t="s">
-        <v>292</v>
-      </c>
       <c r="F56" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G56">
         <v>150</v>
       </c>
       <c r="H56" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I56">
         <v>0.95</v>
@@ -7364,19 +7358,19 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>292</v>
+      </c>
+      <c r="B57" t="s">
+        <v>293</v>
+      </c>
+      <c r="C57" t="s">
         <v>294</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>295</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>296</v>
-      </c>
-      <c r="D57" t="s">
-        <v>297</v>
-      </c>
-      <c r="E57" t="s">
-        <v>298</v>
       </c>
       <c r="F57" t="s">
         <v>141</v>
@@ -7385,7 +7379,7 @@
         <v>200</v>
       </c>
       <c r="H57" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I57">
         <v>0.21</v>
@@ -7436,19 +7430,19 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>298</v>
+      </c>
+      <c r="B58" t="s">
+        <v>299</v>
+      </c>
+      <c r="C58" t="s">
         <v>300</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>301</v>
       </c>
-      <c r="C58" t="s">
+      <c r="E58" t="s">
         <v>302</v>
-      </c>
-      <c r="D58" t="s">
-        <v>303</v>
-      </c>
-      <c r="E58" t="s">
-        <v>304</v>
       </c>
       <c r="F58" t="s">
         <v>141</v>
@@ -7508,19 +7502,19 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>303</v>
+      </c>
+      <c r="B59" t="s">
+        <v>304</v>
+      </c>
+      <c r="C59" t="s">
         <v>305</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>306</v>
       </c>
-      <c r="C59" t="s">
+      <c r="E59" t="s">
         <v>307</v>
-      </c>
-      <c r="D59" t="s">
-        <v>308</v>
-      </c>
-      <c r="E59" t="s">
-        <v>309</v>
       </c>
       <c r="F59" t="s">
         <v>141</v>
@@ -7580,19 +7574,19 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>308</v>
+      </c>
+      <c r="B60" t="s">
+        <v>309</v>
+      </c>
+      <c r="C60" t="s">
         <v>310</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
         <v>311</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>312</v>
-      </c>
-      <c r="D60" t="s">
-        <v>313</v>
-      </c>
-      <c r="E60" t="s">
-        <v>314</v>
       </c>
       <c r="F60" t="s">
         <v>141</v>
@@ -7652,19 +7646,19 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>313</v>
+      </c>
+      <c r="B61" t="s">
+        <v>314</v>
+      </c>
+      <c r="C61" t="s">
         <v>315</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>316</v>
       </c>
-      <c r="C61" t="s">
+      <c r="E61" t="s">
         <v>317</v>
-      </c>
-      <c r="D61" t="s">
-        <v>318</v>
-      </c>
-      <c r="E61" t="s">
-        <v>319</v>
       </c>
       <c r="F61" t="s">
         <v>141</v>
@@ -7673,7 +7667,7 @@
         <v>200</v>
       </c>
       <c r="H61" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I61">
         <v>0.16</v>
@@ -7724,19 +7718,19 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>318</v>
+      </c>
+      <c r="B62" t="s">
+        <v>319</v>
+      </c>
+      <c r="C62" t="s">
         <v>320</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
         <v>321</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E62" t="s">
         <v>322</v>
-      </c>
-      <c r="D62" t="s">
-        <v>323</v>
-      </c>
-      <c r="E62" t="s">
-        <v>324</v>
       </c>
       <c r="F62" t="s">
         <v>141</v>
@@ -7796,19 +7790,19 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>323</v>
+      </c>
+      <c r="B63" t="s">
+        <v>324</v>
+      </c>
+      <c r="C63" t="s">
         <v>325</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>326</v>
       </c>
-      <c r="C63" t="s">
+      <c r="E63" t="s">
         <v>327</v>
-      </c>
-      <c r="D63" t="s">
-        <v>328</v>
-      </c>
-      <c r="E63" t="s">
-        <v>329</v>
       </c>
       <c r="F63" t="s">
         <v>141</v>
@@ -7868,25 +7862,25 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>328</v>
+      </c>
+      <c r="B64" t="s">
+        <v>329</v>
+      </c>
+      <c r="D64" t="s">
         <v>330</v>
       </c>
-      <c r="B64" t="s">
+      <c r="E64" t="s">
         <v>331</v>
       </c>
-      <c r="D64" t="s">
-        <v>332</v>
-      </c>
-      <c r="E64" t="s">
-        <v>333</v>
-      </c>
       <c r="F64" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G64">
         <v>130</v>
       </c>
       <c r="H64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I64">
         <v>1.04</v>
@@ -7937,19 +7931,19 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>332</v>
+      </c>
+      <c r="B65" t="s">
+        <v>333</v>
+      </c>
+      <c r="C65" t="s">
         <v>334</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>335</v>
       </c>
-      <c r="C65" t="s">
+      <c r="E65" t="s">
         <v>336</v>
-      </c>
-      <c r="D65" t="s">
-        <v>337</v>
-      </c>
-      <c r="E65" t="s">
-        <v>338</v>
       </c>
       <c r="F65" t="s">
         <v>148</v>
@@ -8009,19 +8003,19 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>337</v>
+      </c>
+      <c r="B66" t="s">
+        <v>338</v>
+      </c>
+      <c r="C66" t="s">
         <v>339</v>
       </c>
-      <c r="B66" t="s">
+      <c r="D66" t="s">
         <v>340</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>341</v>
-      </c>
-      <c r="D66" t="s">
-        <v>342</v>
-      </c>
-      <c r="E66" t="s">
-        <v>343</v>
       </c>
       <c r="F66" t="s">
         <v>141</v>
@@ -8081,19 +8075,19 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>342</v>
+      </c>
+      <c r="B67" t="s">
+        <v>343</v>
+      </c>
+      <c r="C67" t="s">
         <v>344</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>345</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>346</v>
-      </c>
-      <c r="D67" t="s">
-        <v>347</v>
-      </c>
-      <c r="E67" t="s">
-        <v>348</v>
       </c>
       <c r="F67" t="s">
         <v>141</v>
@@ -8153,19 +8147,19 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>347</v>
+      </c>
+      <c r="B68" t="s">
+        <v>348</v>
+      </c>
+      <c r="C68" t="s">
         <v>349</v>
       </c>
-      <c r="B68" t="s">
+      <c r="D68" t="s">
         <v>350</v>
       </c>
-      <c r="C68" t="s">
+      <c r="E68" t="s">
         <v>351</v>
-      </c>
-      <c r="D68" t="s">
-        <v>352</v>
-      </c>
-      <c r="E68" t="s">
-        <v>353</v>
       </c>
       <c r="F68" t="s">
         <v>141</v>
@@ -8225,7 +8219,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B69" t="s">
         <v>32</v>
@@ -8297,28 +8291,28 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B70" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C70" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D70" t="s">
+        <v>356</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F70" t="s">
         <v>358</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="F70" t="s">
-        <v>360</v>
       </c>
       <c r="G70">
         <v>140</v>
       </c>
       <c r="H70" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I70">
         <v>1.4</v>
@@ -8362,22 +8356,22 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>380</v>
+      </c>
+      <c r="B71" t="s">
+        <v>383</v>
+      </c>
+      <c r="C71" t="s">
         <v>382</v>
       </c>
-      <c r="B71" t="s">
-        <v>385</v>
-      </c>
-      <c r="C71" t="s">
-        <v>384</v>
-      </c>
       <c r="D71" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F71" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G71">
         <v>94</v>
@@ -8427,28 +8421,28 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>386</v>
+      </c>
+      <c r="B72" t="s">
+        <v>387</v>
+      </c>
+      <c r="C72" t="s">
         <v>388</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D72" t="s">
         <v>389</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>390</v>
       </c>
-      <c r="D72" t="s">
-        <v>391</v>
-      </c>
-      <c r="E72" t="s">
-        <v>392</v>
-      </c>
       <c r="F72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G72">
         <v>94</v>
       </c>
       <c r="H72" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I72">
         <v>0.2</v>
@@ -8493,10 +8487,10 @@
         <v>0</v>
       </c>
       <c r="W72" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="X72" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Y72">
         <v>3</v>
@@ -8504,22 +8498,22 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>392</v>
+      </c>
+      <c r="B73" t="s">
+        <v>393</v>
+      </c>
+      <c r="C73" t="s">
         <v>394</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>395</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" t="s">
         <v>396</v>
       </c>
-      <c r="D73" t="s">
-        <v>397</v>
-      </c>
-      <c r="E73" t="s">
-        <v>398</v>
-      </c>
       <c r="F73" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G73">
         <v>94</v>
@@ -8573,7 +8567,7 @@
         <v>11616</v>
       </c>
       <c r="X73" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Y73">
         <v>3</v>
@@ -8581,22 +8575,22 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>397</v>
+      </c>
+      <c r="B74" t="s">
+        <v>398</v>
+      </c>
+      <c r="C74" t="s">
         <v>399</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
         <v>400</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" t="s">
         <v>401</v>
       </c>
-      <c r="D74" t="s">
-        <v>402</v>
-      </c>
-      <c r="E74" t="s">
-        <v>403</v>
-      </c>
       <c r="F74" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G74">
         <v>94</v>
@@ -8650,7 +8644,7 @@
         <v>11616</v>
       </c>
       <c r="X74" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Y74">
         <v>3</v>
@@ -8658,28 +8652,28 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>403</v>
+      </c>
+      <c r="B75" t="s">
+        <v>404</v>
+      </c>
+      <c r="C75" t="s">
         <v>405</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>406</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" t="s">
         <v>407</v>
       </c>
-      <c r="D75" t="s">
+      <c r="F75" t="s">
         <v>408</v>
-      </c>
-      <c r="E75" t="s">
-        <v>409</v>
-      </c>
-      <c r="F75" t="s">
-        <v>410</v>
       </c>
       <c r="G75">
         <v>150</v>
       </c>
       <c r="H75" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I75">
         <v>1.06</v>
@@ -8727,7 +8721,7 @@
         <v>14604</v>
       </c>
       <c r="X75" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Y75">
         <v>3</v>
@@ -8735,28 +8729,28 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>410</v>
+      </c>
+      <c r="B76" t="s">
+        <v>411</v>
+      </c>
+      <c r="C76" t="s">
         <v>412</v>
       </c>
-      <c r="B76" t="s">
+      <c r="D76" t="s">
         <v>413</v>
       </c>
-      <c r="C76" t="s">
+      <c r="E76" t="s">
         <v>414</v>
       </c>
-      <c r="D76" t="s">
-        <v>415</v>
-      </c>
-      <c r="E76" t="s">
-        <v>416</v>
-      </c>
       <c r="F76" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G76">
         <v>150</v>
       </c>
       <c r="H76" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I76">
         <v>1.4</v>
@@ -8801,10 +8795,10 @@
         <v>0</v>
       </c>
       <c r="W76" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="X76" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="Y76">
         <v>3</v>
@@ -8812,19 +8806,19 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>416</v>
+      </c>
+      <c r="B77" t="s">
+        <v>417</v>
+      </c>
+      <c r="C77" t="s">
         <v>418</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>419</v>
       </c>
-      <c r="C77" t="s">
+      <c r="E77" t="s">
         <v>420</v>
-      </c>
-      <c r="D77" t="s">
-        <v>421</v>
-      </c>
-      <c r="E77" t="s">
-        <v>422</v>
       </c>
       <c r="F77" t="s">
         <v>141</v>
@@ -8833,7 +8827,7 @@
         <v>200</v>
       </c>
       <c r="H77" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I77">
         <v>1.4</v>
@@ -8881,7 +8875,7 @@
         <v>14604</v>
       </c>
       <c r="X77" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Y77">
         <v>3</v>
@@ -8889,28 +8883,28 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>421</v>
+      </c>
+      <c r="B78" t="s">
+        <v>422</v>
+      </c>
+      <c r="C78" t="s">
         <v>423</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>424</v>
       </c>
-      <c r="C78" t="s">
+      <c r="E78" t="s">
         <v>425</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" t="s">
         <v>426</v>
-      </c>
-      <c r="E78" t="s">
-        <v>427</v>
-      </c>
-      <c r="F78" t="s">
-        <v>428</v>
       </c>
       <c r="G78">
         <v>150</v>
       </c>
       <c r="H78" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I78">
         <v>1.4</v>
@@ -8955,10 +8949,10 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="X78" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="Y78">
         <v>3</v>
@@ -8966,28 +8960,28 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>427</v>
+      </c>
+      <c r="B79" t="s">
+        <v>428</v>
+      </c>
+      <c r="C79" t="s">
         <v>429</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>430</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
         <v>431</v>
       </c>
-      <c r="D79" t="s">
-        <v>432</v>
-      </c>
-      <c r="E79" t="s">
-        <v>433</v>
-      </c>
       <c r="F79" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G79">
         <v>114</v>
       </c>
       <c r="H79" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I79">
         <v>2.5299999999999998</v>
@@ -9032,10 +9026,10 @@
         <v>0</v>
       </c>
       <c r="W79" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="X79" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="Y79">
         <v>3</v>
@@ -9043,19 +9037,19 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>435</v>
+      </c>
+      <c r="B80" t="s">
+        <v>436</v>
+      </c>
+      <c r="C80" t="s">
         <v>437</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>438</v>
       </c>
-      <c r="C80" t="s">
+      <c r="E80" t="s">
         <v>439</v>
-      </c>
-      <c r="D80" t="s">
-        <v>440</v>
-      </c>
-      <c r="E80" t="s">
-        <v>441</v>
       </c>
       <c r="F80" t="s">
         <v>134</v>
@@ -9064,7 +9058,7 @@
         <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="I80">
         <v>0.67</v>
@@ -9112,7 +9106,7 @@
         <v>14193</v>
       </c>
       <c r="X80" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="Y80">
         <v>3</v>
@@ -9120,19 +9114,19 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>441</v>
+      </c>
+      <c r="B81" t="s">
+        <v>442</v>
+      </c>
+      <c r="C81" t="s">
         <v>443</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>444</v>
       </c>
-      <c r="C81" t="s">
+      <c r="E81" t="s">
         <v>445</v>
-      </c>
-      <c r="D81" t="s">
-        <v>446</v>
-      </c>
-      <c r="E81" t="s">
-        <v>447</v>
       </c>
       <c r="F81" t="s">
         <v>134</v>
@@ -9141,7 +9135,7 @@
         <v>160</v>
       </c>
       <c r="H81" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I81">
         <v>1.4</v>
@@ -9186,10 +9180,10 @@
         <v>0</v>
       </c>
       <c r="W81" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="X81" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="Y81">
         <v>3</v>
@@ -9197,19 +9191,19 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>448</v>
+      </c>
+      <c r="B82" t="s">
+        <v>447</v>
+      </c>
+      <c r="C82" t="s">
+        <v>456</v>
+      </c>
+      <c r="D82" t="s">
+        <v>449</v>
+      </c>
+      <c r="E82" t="s">
         <v>450</v>
-      </c>
-      <c r="B82" t="s">
-        <v>449</v>
-      </c>
-      <c r="C82" t="s">
-        <v>458</v>
-      </c>
-      <c r="D82" t="s">
-        <v>451</v>
-      </c>
-      <c r="E82" t="s">
-        <v>452</v>
       </c>
       <c r="F82" t="s">
         <v>134</v>
@@ -9218,7 +9212,7 @@
         <v>160</v>
       </c>
       <c r="H82" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I82">
         <v>1.62</v>
@@ -9266,7 +9260,7 @@
         <v>11616</v>
       </c>
       <c r="X82" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="Y82">
         <v>3</v>
@@ -9274,28 +9268,28 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>472</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C83" t="s">
         <v>474</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="D83" t="s">
         <v>475</v>
       </c>
-      <c r="C83" t="s">
+      <c r="E83" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="D83" t="s">
-        <v>477</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>478</v>
-      </c>
       <c r="F83" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G83">
         <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I83">
         <v>1.1000000000000001</v>
@@ -9337,10 +9331,10 @@
         <v>0</v>
       </c>
       <c r="W83" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="X83" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="Y83">
         <v>3</v>
@@ -9348,28 +9342,28 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>479</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C84" t="s">
         <v>481</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="D84" t="s">
         <v>482</v>
       </c>
-      <c r="C84" t="s">
+      <c r="E84" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="D84" t="s">
-        <v>484</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>485</v>
-      </c>
       <c r="F84" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G84">
         <v>140</v>
       </c>
       <c r="H84" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I84">
         <v>1.3</v>
@@ -9408,10 +9402,10 @@
         <v>0</v>
       </c>
       <c r="W84" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="X84" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="Y84">
         <v>3</v>
@@ -9419,19 +9413,19 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>486</v>
+      </c>
+      <c r="B85" t="s">
+        <v>487</v>
+      </c>
+      <c r="D85" t="s">
         <v>488</v>
       </c>
-      <c r="B85" t="s">
+      <c r="E85" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="D85" t="s">
-        <v>490</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>491</v>
-      </c>
       <c r="F85" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G85">
         <v>140</v>
@@ -9476,10 +9470,10 @@
         <v>0</v>
       </c>
       <c r="W85" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="X85" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Y85">
         <v>3</v>
@@ -9487,22 +9481,22 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>491</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C86" t="s">
         <v>493</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="D86" t="s">
         <v>494</v>
       </c>
-      <c r="C86" t="s">
+      <c r="E86" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="D86" t="s">
-        <v>496</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>497</v>
-      </c>
       <c r="F86" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G86">
         <v>140</v>
@@ -9553,10 +9547,10 @@
         <v>0</v>
       </c>
       <c r="W86" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="X86" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="Y86">
         <v>3</v>
@@ -9564,19 +9558,19 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>498</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D87" t="s">
         <v>500</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="E87" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="D87" t="s">
-        <v>502</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>503</v>
-      </c>
       <c r="F87" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G87">
         <v>140</v>
@@ -9627,10 +9621,10 @@
         <v>0</v>
       </c>
       <c r="W87" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="X87" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="Y87">
         <v>3</v>
@@ -9638,16 +9632,16 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D88" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F88" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G88">
         <v>140</v>
@@ -9695,7 +9689,7 @@
         <v>11616</v>
       </c>
       <c r="X88" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Y88">
         <v>3</v>
@@ -9703,22 +9697,22 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>507</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="C89" t="s">
+        <v>510</v>
+      </c>
+      <c r="D89" t="s">
         <v>511</v>
       </c>
-      <c r="C89" t="s">
+      <c r="E89" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="D89" t="s">
-        <v>513</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>514</v>
-      </c>
       <c r="F89" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G89">
         <v>140</v>
@@ -9769,10 +9763,10 @@
         <v>0</v>
       </c>
       <c r="W89" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="X89" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="Y89">
         <v>3</v>
@@ -9780,22 +9774,22 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>513</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="C90" t="s">
+        <v>521</v>
+      </c>
+      <c r="D90" t="s">
+        <v>514</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="B90" s="7" t="s">
-        <v>522</v>
-      </c>
-      <c r="C90" t="s">
-        <v>523</v>
-      </c>
-      <c r="D90" t="s">
-        <v>516</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>517</v>
-      </c>
       <c r="F90" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G90">
         <v>140</v>
@@ -9849,7 +9843,7 @@
         <v>11616</v>
       </c>
       <c r="X90" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Y90">
         <v>3</v>
@@ -9857,25 +9851,25 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>516</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="B91" s="7" t="s">
-        <v>520</v>
-      </c>
       <c r="C91" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D91" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F91" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G91">
         <v>140</v>
       </c>
       <c r="H91" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I91">
         <v>0.9</v>
@@ -9920,10 +9914,10 @@
         <v>0</v>
       </c>
       <c r="W91" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="X91" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="Y91">
         <v>3</v>

</xml_diff>

<commit_message>
updates to full sample excel file
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7B2F1-79E5-8A4C-B93D-0FAAEF330A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D48B7-878C-D145-925B-B3B8BC22047A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8120" yWindow="460" windowWidth="29640" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="525">
   <si>
     <t>2MASS</t>
   </si>
@@ -130,9 +130,6 @@
     <t>-2d45m09.7s</t>
   </si>
   <si>
-    <t>sigma Ori</t>
-  </si>
-  <si>
     <t>K6.0</t>
   </si>
   <si>
@@ -1102,9 +1099,6 @@
     <t>08h42m38.78s</t>
   </si>
   <si>
-    <t>Eta Cha</t>
-  </si>
-  <si>
     <t>PID</t>
   </si>
   <si>
@@ -1384,9 +1378,6 @@
     <t>COS/G160M</t>
   </si>
   <si>
-    <t>Eps Cha</t>
-  </si>
-  <si>
     <t>DR</t>
   </si>
   <si>
@@ -1592,6 +1583,18 @@
   </si>
   <si>
     <t>COS/G130M/G160M</t>
+  </si>
+  <si>
+    <t>Sigma Ori</t>
+  </si>
+  <si>
+    <t>eta Cha</t>
+  </si>
+  <si>
+    <t>eps Cha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sigma Ori </t>
   </si>
 </sst>
 </file>
@@ -3167,8 +3170,8 @@
   <dimension ref="A1:Y91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3184,7 +3187,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3223,16 +3226,16 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>353</v>
+      </c>
+      <c r="O1" t="s">
+        <v>351</v>
+      </c>
+      <c r="P1" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q1" t="s">
         <v>354</v>
-      </c>
-      <c r="O1" t="s">
-        <v>352</v>
-      </c>
-      <c r="P1" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>355</v>
       </c>
       <c r="R1" t="s">
         <v>12</v>
@@ -3241,22 +3244,22 @@
         <v>13</v>
       </c>
       <c r="T1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="U1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="V1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="W1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="X1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="Y1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3334,7 +3337,7 @@
         <v>16115</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="Y2">
         <v>2</v>
@@ -3498,7 +3501,7 @@
     </row>
     <row r="5" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -3513,13 +3516,13 @@
         <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>521</v>
       </c>
       <c r="G5" s="1">
         <v>385</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="1">
         <v>0.754</v>
@@ -3577,28 +3580,28 @@
     </row>
     <row r="6" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>521</v>
       </c>
       <c r="G6" s="1">
         <v>385</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="1">
         <v>1.087</v>
@@ -3656,17 +3659,17 @@
     </row>
     <row r="7" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
@@ -3733,26 +3736,26 @@
     </row>
     <row r="8" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="G8" s="1">
         <v>330</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="1">
         <v>0.34</v>
@@ -3810,28 +3813,28 @@
     </row>
     <row r="9" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>521</v>
       </c>
       <c r="G9" s="1">
         <v>385</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I9" s="1">
         <v>0.875</v>
@@ -3889,17 +3892,17 @@
     </row>
     <row r="10" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>19</v>
@@ -3966,17 +3969,17 @@
     </row>
     <row r="11" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
@@ -4043,19 +4046,19 @@
     </row>
     <row r="12" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>19</v>
@@ -4064,7 +4067,7 @@
         <v>440</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1">
         <v>0.35</v>
@@ -4122,17 +4125,17 @@
     </row>
     <row r="13" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>19</v>
@@ -4193,7 +4196,7 @@
         <v>16114</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="Y13">
         <v>2</v>
@@ -4201,26 +4204,26 @@
     </row>
     <row r="14" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="1">
         <v>330</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I14" s="1">
         <v>0.33</v>
@@ -4278,28 +4281,28 @@
     </row>
     <row r="15" spans="1:25" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="G15" s="2">
         <v>46</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I15" s="2">
         <v>0.28999999999999998</v>
@@ -4352,22 +4355,22 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="G16" s="6">
         <v>150</v>
@@ -4428,22 +4431,22 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="6">
         <v>150</v>
@@ -4504,28 +4507,28 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G18" s="6">
         <v>150</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I18" s="6">
         <v>0.37</v>
@@ -4580,28 +4583,28 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="F19" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19" s="6">
         <v>150</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I19" s="6">
         <v>0.2</v>
@@ -4656,26 +4659,26 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>110</v>
-      </c>
       <c r="F20" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="6">
         <v>150</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I20" s="6">
         <v>0.23</v>
@@ -4730,28 +4733,28 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="F21" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" s="6">
         <v>150</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I21" s="6">
         <v>0.42</v>
@@ -4806,28 +4809,28 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>122</v>
-      </c>
       <c r="F22" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G22" s="6">
         <v>150</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I22" s="6">
         <v>0.28999999999999998</v>
@@ -4882,28 +4885,28 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>124</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>125</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>126</v>
       </c>
-      <c r="E23" t="s">
-        <v>127</v>
-      </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G23">
         <v>150</v>
       </c>
       <c r="H23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I23">
         <v>0.3</v>
@@ -4954,28 +4957,28 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="G24" s="6">
         <v>160</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I24" s="6">
         <v>0.16</v>
@@ -5026,28 +5029,28 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="G25" s="6">
         <v>200</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I25" s="6">
         <v>0.47</v>
@@ -5102,28 +5105,28 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="G26" s="6">
         <v>150</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I26" s="6">
         <v>0.41</v>
@@ -5178,28 +5181,28 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>152</v>
-      </c>
       <c r="F27" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G27" s="6">
         <v>160</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I27" s="6">
         <v>0.17</v>
@@ -5250,28 +5253,28 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="F28" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G28" s="6">
         <v>150</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I28" s="6">
         <v>0.2</v>
@@ -5326,28 +5329,28 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" t="s">
         <v>158</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>159</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>160</v>
       </c>
-      <c r="E29" t="s">
-        <v>161</v>
-      </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29">
         <v>160</v>
       </c>
       <c r="H29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I29">
         <v>0.3</v>
@@ -5398,28 +5401,28 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="F30" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G30" s="6">
         <v>200</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I30" s="6">
         <v>0.16</v>
@@ -5474,28 +5477,28 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" t="s">
         <v>167</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>168</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>169</v>
       </c>
-      <c r="E31" t="s">
-        <v>170</v>
-      </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G31">
         <v>160</v>
       </c>
       <c r="H31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I31">
         <v>0.49</v>
@@ -5546,28 +5549,28 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" t="s">
         <v>172</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>173</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>174</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>175</v>
       </c>
-      <c r="E32" t="s">
-        <v>176</v>
-      </c>
       <c r="F32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G32">
         <v>200</v>
       </c>
       <c r="H32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I32">
         <v>0.44</v>
@@ -5618,25 +5621,25 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" t="s">
         <v>177</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>178</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>179</v>
       </c>
-      <c r="E33" t="s">
-        <v>180</v>
-      </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G33">
         <v>160</v>
       </c>
       <c r="H33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I33">
         <v>0.2</v>
@@ -5687,28 +5690,28 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="F34" s="3" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G34" s="3">
         <v>94</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I34" s="3">
         <v>0.15</v>
@@ -5759,28 +5762,28 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G35" s="3">
         <v>94</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I35" s="3">
         <v>0.15</v>
@@ -5831,28 +5834,28 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="F36" s="6" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G36" s="6">
         <v>94</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I36" s="6">
         <v>5.1999999999999998E-2</v>
@@ -5907,28 +5910,28 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G37" s="2">
         <v>94</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I37" s="2">
         <v>0.78</v>
@@ -5981,28 +5984,28 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G38" s="2">
         <v>94</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I38" s="2">
         <v>0.28999999999999998</v>
@@ -6055,28 +6058,28 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B39" t="s">
         <v>203</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>204</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>205</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>206</v>
       </c>
-      <c r="E39" t="s">
-        <v>207</v>
-      </c>
       <c r="F39" t="s">
-        <v>454</v>
+        <v>523</v>
       </c>
       <c r="G39">
         <v>160</v>
       </c>
       <c r="H39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I39">
         <v>0.19</v>
@@ -6121,28 +6124,28 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>212</v>
-      </c>
       <c r="F40" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G40" s="6">
         <v>160</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I40" s="6">
         <v>0.14000000000000001</v>
@@ -6193,26 +6196,26 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>217</v>
-      </c>
       <c r="F41" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G41" s="6">
         <v>160</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I41" s="6">
         <v>1.25</v>
@@ -6267,28 +6270,28 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>223</v>
-      </c>
       <c r="F42" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G42" s="6">
         <v>160</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I42" s="6">
         <v>0.51</v>
@@ -6340,33 +6343,33 @@
         <v>16482</v>
       </c>
       <c r="X42" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>227</v>
-      </c>
       <c r="F43" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G43" s="6">
         <v>160</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I43" s="6">
         <v>0.19</v>
@@ -6421,22 +6424,22 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" t="s">
         <v>228</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>229</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>230</v>
       </c>
-      <c r="E44" t="s">
-        <v>231</v>
-      </c>
       <c r="F44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G44">
         <v>160</v>
@@ -6493,28 +6496,28 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>236</v>
-      </c>
       <c r="F45" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G45" s="6">
         <v>160</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I45" s="6">
         <v>0.25</v>
@@ -6569,28 +6572,28 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B46" t="s">
+        <v>236</v>
+      </c>
+      <c r="C46" t="s">
         <v>237</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>238</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>239</v>
       </c>
-      <c r="E46" t="s">
-        <v>240</v>
-      </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G46">
         <v>160</v>
       </c>
       <c r="H46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I46">
         <v>1.31</v>
@@ -6641,22 +6644,22 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B47" t="s">
+        <v>240</v>
+      </c>
+      <c r="C47" t="s">
         <v>241</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>242</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>243</v>
       </c>
-      <c r="E47" t="s">
-        <v>244</v>
-      </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G47">
         <v>160</v>
@@ -6713,28 +6716,28 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>244</v>
+      </c>
+      <c r="B48" t="s">
         <v>245</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>246</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>247</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>248</v>
       </c>
-      <c r="E48" t="s">
-        <v>249</v>
-      </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G48">
         <v>160</v>
       </c>
       <c r="H48" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I48">
         <v>2.08</v>
@@ -6785,28 +6788,28 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B49" t="s">
+        <v>250</v>
+      </c>
+      <c r="C49" t="s">
         <v>251</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>252</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>253</v>
       </c>
-      <c r="E49" t="s">
-        <v>254</v>
-      </c>
       <c r="F49" t="s">
-        <v>454</v>
+        <v>523</v>
       </c>
       <c r="G49">
         <v>114</v>
       </c>
       <c r="H49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I49">
         <v>0.9</v>
@@ -6857,28 +6860,28 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B50" t="s">
+        <v>254</v>
+      </c>
+      <c r="C50" t="s">
         <v>255</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>256</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>257</v>
       </c>
-      <c r="E50" t="s">
-        <v>258</v>
-      </c>
       <c r="F50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G50">
         <v>160</v>
       </c>
       <c r="H50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I50">
         <v>0.1</v>
@@ -6929,28 +6932,28 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" t="s">
         <v>260</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>261</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>262</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>263</v>
       </c>
-      <c r="E51" t="s">
-        <v>264</v>
-      </c>
       <c r="F51" t="s">
-        <v>454</v>
+        <v>523</v>
       </c>
       <c r="G51">
         <v>114</v>
       </c>
       <c r="H51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I51">
         <v>0.16</v>
@@ -7001,28 +7004,28 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>264</v>
+      </c>
+      <c r="B52" t="s">
         <v>265</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>266</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>267</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>268</v>
       </c>
-      <c r="E52" t="s">
-        <v>269</v>
-      </c>
       <c r="F52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G52">
         <v>200</v>
       </c>
       <c r="H52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I52">
         <v>0.22</v>
@@ -7073,28 +7076,28 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>269</v>
+      </c>
+      <c r="B53" t="s">
         <v>270</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>271</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>272</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>273</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>274</v>
-      </c>
-      <c r="F53" t="s">
-        <v>275</v>
       </c>
       <c r="G53">
         <v>130</v>
       </c>
       <c r="H53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I53">
         <v>0.93</v>
@@ -7145,25 +7148,25 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>275</v>
+      </c>
+      <c r="B54" t="s">
         <v>276</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>277</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>278</v>
       </c>
-      <c r="E54" t="s">
-        <v>279</v>
-      </c>
       <c r="F54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G54">
         <v>150</v>
       </c>
       <c r="H54" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I54">
         <v>0.16</v>
@@ -7214,28 +7217,28 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>279</v>
+      </c>
+      <c r="B55" t="s">
         <v>280</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>281</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>282</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>283</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>284</v>
-      </c>
-      <c r="F55" t="s">
-        <v>285</v>
       </c>
       <c r="G55">
         <v>150</v>
       </c>
       <c r="H55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I55">
         <v>0.5</v>
@@ -7286,28 +7289,28 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>285</v>
+      </c>
+      <c r="B56" t="s">
         <v>286</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>287</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>288</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>289</v>
       </c>
-      <c r="E56" t="s">
-        <v>290</v>
-      </c>
       <c r="F56" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G56">
         <v>150</v>
       </c>
       <c r="H56" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I56">
         <v>0.95</v>
@@ -7358,28 +7361,28 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>291</v>
+      </c>
+      <c r="B57" t="s">
         <v>292</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>293</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>294</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>295</v>
       </c>
-      <c r="E57" t="s">
-        <v>296</v>
-      </c>
       <c r="F57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G57">
         <v>200</v>
       </c>
       <c r="H57" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I57">
         <v>0.21</v>
@@ -7430,28 +7433,28 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>297</v>
+      </c>
+      <c r="B58" t="s">
         <v>298</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>299</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>300</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>301</v>
       </c>
-      <c r="E58" t="s">
-        <v>302</v>
-      </c>
       <c r="F58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G58">
         <v>200</v>
       </c>
       <c r="H58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I58">
         <v>0.23</v>
@@ -7502,28 +7505,28 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>302</v>
+      </c>
+      <c r="B59" t="s">
         <v>303</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>304</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>305</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>306</v>
       </c>
-      <c r="E59" t="s">
-        <v>307</v>
-      </c>
       <c r="F59" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G59">
         <v>200</v>
       </c>
       <c r="H59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I59">
         <v>0.26</v>
@@ -7574,28 +7577,28 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>307</v>
+      </c>
+      <c r="B60" t="s">
         <v>308</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>309</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>310</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>311</v>
       </c>
-      <c r="E60" t="s">
-        <v>312</v>
-      </c>
       <c r="F60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G60">
         <v>200</v>
       </c>
       <c r="H60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I60">
         <v>0.23</v>
@@ -7646,28 +7649,28 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>312</v>
+      </c>
+      <c r="B61" t="s">
         <v>313</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>314</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>315</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>316</v>
       </c>
-      <c r="E61" t="s">
-        <v>317</v>
-      </c>
       <c r="F61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G61">
         <v>200</v>
       </c>
       <c r="H61" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I61">
         <v>0.16</v>
@@ -7718,22 +7721,22 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>317</v>
+      </c>
+      <c r="B62" t="s">
         <v>318</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>319</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>320</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>321</v>
       </c>
-      <c r="E62" t="s">
-        <v>322</v>
-      </c>
       <c r="F62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G62">
         <v>200</v>
@@ -7790,28 +7793,28 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>322</v>
+      </c>
+      <c r="B63" t="s">
         <v>323</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>324</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>325</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>326</v>
       </c>
-      <c r="E63" t="s">
-        <v>327</v>
-      </c>
       <c r="F63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G63">
         <v>200</v>
       </c>
       <c r="H63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I63">
         <v>0.17</v>
@@ -7862,25 +7865,25 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>327</v>
+      </c>
+      <c r="B64" t="s">
         <v>328</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>329</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>330</v>
       </c>
-      <c r="E64" t="s">
-        <v>331</v>
-      </c>
       <c r="F64" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G64">
         <v>130</v>
       </c>
       <c r="H64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I64">
         <v>1.04</v>
@@ -7931,22 +7934,22 @@
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>331</v>
+      </c>
+      <c r="B65" t="s">
         <v>332</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>333</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>334</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>335</v>
       </c>
-      <c r="E65" t="s">
-        <v>336</v>
-      </c>
       <c r="F65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G65">
         <v>150</v>
@@ -8003,28 +8006,28 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>336</v>
+      </c>
+      <c r="B66" t="s">
         <v>337</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>338</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>339</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>340</v>
       </c>
-      <c r="E66" t="s">
-        <v>341</v>
-      </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G66">
         <v>200</v>
       </c>
       <c r="H66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I66">
         <v>0.16</v>
@@ -8075,28 +8078,28 @@
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>341</v>
+      </c>
+      <c r="B67" t="s">
         <v>342</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>343</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>344</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>345</v>
       </c>
-      <c r="E67" t="s">
-        <v>346</v>
-      </c>
       <c r="F67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G67">
         <v>200</v>
       </c>
       <c r="H67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I67">
         <v>0.22</v>
@@ -8147,28 +8150,28 @@
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>346</v>
+      </c>
+      <c r="B68" t="s">
         <v>347</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>348</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>349</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>350</v>
       </c>
-      <c r="E68" t="s">
-        <v>351</v>
-      </c>
       <c r="F68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G68">
         <v>200</v>
       </c>
       <c r="H68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I68">
         <v>0.19</v>
@@ -8219,7 +8222,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B69" t="s">
         <v>32</v>
@@ -8234,13 +8237,13 @@
         <v>35</v>
       </c>
       <c r="F69" t="s">
-        <v>36</v>
+        <v>524</v>
       </c>
       <c r="G69">
         <v>385</v>
       </c>
       <c r="H69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I69">
         <v>0.754</v>
@@ -8291,28 +8294,28 @@
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B70" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C70" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D70" t="s">
+        <v>355</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="F70" t="s">
         <v>357</v>
-      </c>
-      <c r="F70" t="s">
-        <v>358</v>
       </c>
       <c r="G70">
         <v>140</v>
       </c>
       <c r="H70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I70">
         <v>1.4</v>
@@ -8356,28 +8359,28 @@
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>378</v>
+      </c>
+      <c r="B71" t="s">
+        <v>381</v>
+      </c>
+      <c r="C71" t="s">
         <v>380</v>
       </c>
-      <c r="B71" t="s">
-        <v>383</v>
-      </c>
-      <c r="C71" t="s">
-        <v>382</v>
-      </c>
       <c r="D71" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="F71" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G71">
         <v>94</v>
       </c>
       <c r="H71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I71">
         <v>0.3</v>
@@ -8421,28 +8424,28 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>384</v>
+      </c>
+      <c r="B72" t="s">
+        <v>385</v>
+      </c>
+      <c r="C72" t="s">
         <v>386</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D72" t="s">
         <v>387</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>388</v>
       </c>
-      <c r="D72" t="s">
-        <v>389</v>
-      </c>
-      <c r="E72" t="s">
-        <v>390</v>
-      </c>
       <c r="F72" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G72">
         <v>94</v>
       </c>
       <c r="H72" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I72">
         <v>0.2</v>
@@ -8487,10 +8490,10 @@
         <v>0</v>
       </c>
       <c r="W72" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="X72" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="Y72">
         <v>3</v>
@@ -8498,28 +8501,28 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>390</v>
+      </c>
+      <c r="B73" t="s">
+        <v>391</v>
+      </c>
+      <c r="C73" t="s">
         <v>392</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>393</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" t="s">
         <v>394</v>
       </c>
-      <c r="D73" t="s">
-        <v>395</v>
-      </c>
-      <c r="E73" t="s">
-        <v>396</v>
-      </c>
       <c r="F73" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G73">
         <v>94</v>
       </c>
       <c r="H73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I73">
         <v>0.75</v>
@@ -8567,7 +8570,7 @@
         <v>11616</v>
       </c>
       <c r="X73" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="Y73">
         <v>3</v>
@@ -8575,28 +8578,28 @@
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>395</v>
+      </c>
+      <c r="B74" t="s">
+        <v>396</v>
+      </c>
+      <c r="C74" t="s">
         <v>397</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
         <v>398</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" t="s">
         <v>399</v>
       </c>
-      <c r="D74" t="s">
-        <v>400</v>
-      </c>
-      <c r="E74" t="s">
-        <v>401</v>
-      </c>
       <c r="F74" t="s">
-        <v>360</v>
+        <v>522</v>
       </c>
       <c r="G74">
         <v>94</v>
       </c>
       <c r="H74" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I74">
         <v>0.83</v>
@@ -8644,7 +8647,7 @@
         <v>11616</v>
       </c>
       <c r="X74" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="Y74">
         <v>3</v>
@@ -8652,28 +8655,28 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>401</v>
+      </c>
+      <c r="B75" t="s">
+        <v>402</v>
+      </c>
+      <c r="C75" t="s">
         <v>403</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>404</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" t="s">
         <v>405</v>
       </c>
-      <c r="D75" t="s">
+      <c r="F75" t="s">
         <v>406</v>
-      </c>
-      <c r="E75" t="s">
-        <v>407</v>
-      </c>
-      <c r="F75" t="s">
-        <v>408</v>
       </c>
       <c r="G75">
         <v>150</v>
       </c>
       <c r="H75" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I75">
         <v>1.06</v>
@@ -8721,7 +8724,7 @@
         <v>14604</v>
       </c>
       <c r="X75" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="Y75">
         <v>3</v>
@@ -8729,28 +8732,28 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>408</v>
+      </c>
+      <c r="B76" t="s">
+        <v>409</v>
+      </c>
+      <c r="C76" t="s">
         <v>410</v>
       </c>
-      <c r="B76" t="s">
+      <c r="D76" t="s">
         <v>411</v>
       </c>
-      <c r="C76" t="s">
+      <c r="E76" t="s">
         <v>412</v>
       </c>
-      <c r="D76" t="s">
-        <v>413</v>
-      </c>
-      <c r="E76" t="s">
-        <v>414</v>
-      </c>
       <c r="F76" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G76">
         <v>150</v>
       </c>
       <c r="H76" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I76">
         <v>1.4</v>
@@ -8795,10 +8798,10 @@
         <v>0</v>
       </c>
       <c r="W76" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="X76" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="Y76">
         <v>3</v>
@@ -8806,28 +8809,28 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>414</v>
+      </c>
+      <c r="B77" t="s">
+        <v>415</v>
+      </c>
+      <c r="C77" t="s">
         <v>416</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>417</v>
       </c>
-      <c r="C77" t="s">
+      <c r="E77" t="s">
         <v>418</v>
       </c>
-      <c r="D77" t="s">
-        <v>419</v>
-      </c>
-      <c r="E77" t="s">
-        <v>420</v>
-      </c>
       <c r="F77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G77">
         <v>200</v>
       </c>
       <c r="H77" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I77">
         <v>1.4</v>
@@ -8875,7 +8878,7 @@
         <v>14604</v>
       </c>
       <c r="X77" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="Y77">
         <v>3</v>
@@ -8883,28 +8886,28 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>419</v>
+      </c>
+      <c r="B78" t="s">
+        <v>420</v>
+      </c>
+      <c r="C78" t="s">
         <v>421</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>422</v>
       </c>
-      <c r="C78" t="s">
+      <c r="E78" t="s">
         <v>423</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" t="s">
         <v>424</v>
-      </c>
-      <c r="E78" t="s">
-        <v>425</v>
-      </c>
-      <c r="F78" t="s">
-        <v>426</v>
       </c>
       <c r="G78">
         <v>150</v>
       </c>
       <c r="H78" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I78">
         <v>1.4</v>
@@ -8949,10 +8952,10 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="X78" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="Y78">
         <v>3</v>
@@ -8960,28 +8963,28 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>425</v>
+      </c>
+      <c r="B79" t="s">
+        <v>426</v>
+      </c>
+      <c r="C79" t="s">
         <v>427</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>428</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
         <v>429</v>
       </c>
-      <c r="D79" t="s">
-        <v>430</v>
-      </c>
-      <c r="E79" t="s">
-        <v>431</v>
-      </c>
       <c r="F79" t="s">
-        <v>454</v>
+        <v>523</v>
       </c>
       <c r="G79">
         <v>114</v>
       </c>
       <c r="H79" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I79">
         <v>2.5299999999999998</v>
@@ -9026,10 +9029,10 @@
         <v>0</v>
       </c>
       <c r="W79" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="X79" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="Y79">
         <v>3</v>
@@ -9037,28 +9040,28 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>433</v>
+      </c>
+      <c r="B80" t="s">
+        <v>434</v>
+      </c>
+      <c r="C80" t="s">
         <v>435</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>436</v>
       </c>
-      <c r="C80" t="s">
+      <c r="E80" t="s">
         <v>437</v>
       </c>
-      <c r="D80" t="s">
-        <v>438</v>
-      </c>
-      <c r="E80" t="s">
-        <v>439</v>
-      </c>
       <c r="F80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G80">
         <v>160</v>
       </c>
       <c r="H80" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="I80">
         <v>0.67</v>
@@ -9106,7 +9109,7 @@
         <v>14193</v>
       </c>
       <c r="X80" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Y80">
         <v>3</v>
@@ -9114,28 +9117,28 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>439</v>
+      </c>
+      <c r="B81" t="s">
+        <v>440</v>
+      </c>
+      <c r="C81" t="s">
         <v>441</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>442</v>
       </c>
-      <c r="C81" t="s">
+      <c r="E81" t="s">
         <v>443</v>
       </c>
-      <c r="D81" t="s">
-        <v>444</v>
-      </c>
-      <c r="E81" t="s">
-        <v>445</v>
-      </c>
       <c r="F81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G81">
         <v>160</v>
       </c>
       <c r="H81" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="I81">
         <v>1.4</v>
@@ -9180,10 +9183,10 @@
         <v>0</v>
       </c>
       <c r="W81" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="X81" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="Y81">
         <v>3</v>
@@ -9191,28 +9194,28 @@
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>446</v>
+      </c>
+      <c r="B82" t="s">
+        <v>445</v>
+      </c>
+      <c r="C82" t="s">
+        <v>453</v>
+      </c>
+      <c r="D82" t="s">
+        <v>447</v>
+      </c>
+      <c r="E82" t="s">
         <v>448</v>
       </c>
-      <c r="B82" t="s">
-        <v>447</v>
-      </c>
-      <c r="C82" t="s">
-        <v>456</v>
-      </c>
-      <c r="D82" t="s">
-        <v>449</v>
-      </c>
-      <c r="E82" t="s">
-        <v>450</v>
-      </c>
       <c r="F82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G82">
         <v>160</v>
       </c>
       <c r="H82" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I82">
         <v>1.62</v>
@@ -9260,7 +9263,7 @@
         <v>11616</v>
       </c>
       <c r="X82" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="Y82">
         <v>3</v>
@@ -9268,28 +9271,28 @@
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>469</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C83" t="s">
+        <v>471</v>
+      </c>
+      <c r="D83" t="s">
         <v>472</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="E83" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C83" t="s">
-        <v>474</v>
-      </c>
-      <c r="D83" t="s">
-        <v>475</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>476</v>
-      </c>
       <c r="F83" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G83">
         <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I83">
         <v>1.1000000000000001</v>
@@ -9331,10 +9334,10 @@
         <v>0</v>
       </c>
       <c r="W83" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="X83" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="Y83">
         <v>3</v>
@@ -9342,28 +9345,28 @@
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>476</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="C84" t="s">
+        <v>478</v>
+      </c>
+      <c r="D84" t="s">
         <v>479</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="E84" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="C84" t="s">
-        <v>481</v>
-      </c>
-      <c r="D84" t="s">
-        <v>482</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>483</v>
-      </c>
       <c r="F84" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G84">
         <v>140</v>
       </c>
       <c r="H84" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I84">
         <v>1.3</v>
@@ -9402,10 +9405,10 @@
         <v>0</v>
       </c>
       <c r="W84" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="X84" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="Y84">
         <v>3</v>
@@ -9413,19 +9416,19 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>483</v>
+      </c>
+      <c r="B85" t="s">
+        <v>484</v>
+      </c>
+      <c r="D85" t="s">
+        <v>485</v>
+      </c>
+      <c r="E85" s="4" t="s">
         <v>486</v>
       </c>
-      <c r="B85" t="s">
-        <v>487</v>
-      </c>
-      <c r="D85" t="s">
-        <v>488</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>489</v>
-      </c>
       <c r="F85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G85">
         <v>140</v>
@@ -9470,10 +9473,10 @@
         <v>0</v>
       </c>
       <c r="W85" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="X85" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="Y85">
         <v>3</v>
@@ -9481,22 +9484,22 @@
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>488</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C86" t="s">
+        <v>490</v>
+      </c>
+      <c r="D86" t="s">
         <v>491</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="E86" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="C86" t="s">
-        <v>493</v>
-      </c>
-      <c r="D86" t="s">
-        <v>494</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>495</v>
-      </c>
       <c r="F86" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G86">
         <v>140</v>
@@ -9547,10 +9550,10 @@
         <v>0</v>
       </c>
       <c r="W86" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="X86" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="Y86">
         <v>3</v>
@@ -9558,25 +9561,25 @@
     </row>
     <row r="87" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>495</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="D87" t="s">
+        <v>497</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>499</v>
-      </c>
-      <c r="D87" t="s">
-        <v>500</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>501</v>
-      </c>
       <c r="F87" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G87">
         <v>140</v>
       </c>
       <c r="H87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I87">
         <v>0.4</v>
@@ -9621,10 +9624,10 @@
         <v>0</v>
       </c>
       <c r="W87" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="X87" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="Y87">
         <v>3</v>
@@ -9632,16 +9635,16 @@
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D88" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F88" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G88">
         <v>140</v>
@@ -9689,7 +9692,7 @@
         <v>11616</v>
       </c>
       <c r="X88" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Y88">
         <v>3</v>
@@ -9697,28 +9700,28 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>504</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="C89" t="s">
         <v>507</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="D89" t="s">
+        <v>508</v>
+      </c>
+      <c r="E89" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C89" t="s">
-        <v>510</v>
-      </c>
-      <c r="D89" t="s">
-        <v>511</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>512</v>
-      </c>
       <c r="F89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G89">
         <v>140</v>
       </c>
       <c r="H89" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I89">
         <v>0.5</v>
@@ -9763,10 +9766,10 @@
         <v>0</v>
       </c>
       <c r="W89" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="X89" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="Y89">
         <v>3</v>
@@ -9774,22 +9777,22 @@
     </row>
     <row r="90" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C90" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D90" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F90" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G90">
         <v>140</v>
@@ -9843,7 +9846,7 @@
         <v>11616</v>
       </c>
       <c r="X90" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Y90">
         <v>3</v>
@@ -9851,25 +9854,25 @@
     </row>
     <row r="91" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>513</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="C91" t="s">
         <v>516</v>
       </c>
-      <c r="B91" s="7" t="s">
-        <v>518</v>
-      </c>
-      <c r="C91" t="s">
-        <v>519</v>
-      </c>
       <c r="D91" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F91" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G91">
         <v>140</v>
       </c>
       <c r="H91" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I91">
         <v>0.9</v>
@@ -9914,10 +9917,10 @@
         <v>0</v>
       </c>
       <c r="W91" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="X91" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="Y91">
         <v>3</v>

</xml_diff>

<commit_message>
updated orbit number for WZ Cha
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69D48B7-878C-D145-925B-B3B8BC22047A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33371C83-3D9C-124C-B6AE-E8D41087215C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8120" yWindow="460" windowWidth="29640" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3169,9 +3169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5387,16 +5387,14 @@
         <v>0.36</v>
       </c>
       <c r="T29">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="U29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V29">
-        <f t="shared" si="4"/>
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed COS orbits for V505-Ori
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33371C83-3D9C-124C-B6AE-E8D41087215C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E56A7B-A040-984D-8B83-F7D063AB18CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8120" yWindow="460" windowWidth="29640" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3169,9 +3169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U73" sqref="U73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3559,8 +3559,7 @@
         <v>0.36</v>
       </c>
       <c r="T5" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5" s="1">
         <f t="shared" si="2"/>
@@ -8278,8 +8277,7 @@
         <v>0.36</v>
       </c>
       <c r="T69">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U69">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
Added PIDs for Cy 29 batch; removed 2MASS...5546 (not observing); corrected AA Omega targets names for LMC in alias and target table
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E56A7B-A040-984D-8B83-F7D063AB18CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA581FDD-9B00-8343-879E-ED9DCD2EE181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="460" windowWidth="29640" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8680" yWindow="920" windowWidth="35780" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -1601,7 +1601,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1732,13 +1732,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2092,15 +2085,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="11"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3169,9 +3163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U73" sqref="U73"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4353,534 +4347,534 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>150</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="4">
         <v>0.86</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="4">
         <v>-7.67</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="4">
         <v>0.7</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="4">
         <v>12.19</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="4">
         <v>11.4</v>
       </c>
-      <c r="N16" s="6">
-        <v>1</v>
-      </c>
-      <c r="O16" s="6">
-        <v>1</v>
-      </c>
-      <c r="P16" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="6">
+      <c r="N16" s="4">
+        <v>1</v>
+      </c>
+      <c r="O16" s="4">
+        <v>1</v>
+      </c>
+      <c r="P16" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R16" s="4">
         <v>1.65</v>
       </c>
-      <c r="S16" s="6">
+      <c r="S16" s="4">
         <v>0.23</v>
       </c>
-      <c r="T16" s="6">
+      <c r="T16" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U16" s="6">
+      <c r="U16" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V16" s="6">
+      <c r="V16" s="4">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="W16" s="6">
+      <c r="W16" s="4">
         <v>16476</v>
       </c>
-      <c r="X16" s="6"/>
+      <c r="X16" s="4"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="4">
         <v>150</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="4">
         <v>0.75</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="4">
         <v>-8.7899999999999991</v>
       </c>
-      <c r="K17" s="6">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6">
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
         <v>13.35</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="4">
         <v>13.26</v>
       </c>
-      <c r="N17" s="6">
-        <v>1</v>
-      </c>
-      <c r="O17" s="6">
-        <v>1</v>
-      </c>
-      <c r="P17" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="6">
+      <c r="N17" s="4">
+        <v>1</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17" s="4">
         <v>1.21</v>
       </c>
-      <c r="S17" s="6">
+      <c r="S17" s="4">
         <v>0.22</v>
       </c>
-      <c r="T17" s="6">
+      <c r="T17" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U17" s="6">
+      <c r="U17" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V17" s="6">
+      <c r="V17" s="4">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="W17" s="6">
+      <c r="W17" s="4">
         <v>16476</v>
       </c>
-      <c r="X17" s="6"/>
+      <c r="X17" s="4"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <v>150</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="4">
         <v>0.37</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="4">
         <v>-8.65</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="4">
         <v>0.75</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="4">
         <v>15.15</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="4">
         <v>14.79</v>
       </c>
-      <c r="N18" s="6">
-        <v>1</v>
-      </c>
-      <c r="O18" s="6">
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18" s="4">
         <v>3</v>
       </c>
-      <c r="P18" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="6">
+      <c r="P18" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R18" s="6">
+      <c r="R18" s="4">
         <v>4.9400000000000004</v>
       </c>
-      <c r="S18" s="6">
+      <c r="S18" s="4">
         <v>0.3</v>
       </c>
-      <c r="T18" s="6">
+      <c r="T18" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U18" s="6">
+      <c r="U18" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V18" s="6">
+      <c r="V18" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="W18" s="6">
+      <c r="W18" s="4">
         <v>16477</v>
       </c>
-      <c r="X18" s="6"/>
+      <c r="X18" s="4"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="4">
         <v>150</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="4">
         <v>0.2</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="4">
         <v>-9.51</v>
       </c>
-      <c r="K19" s="6">
-        <v>0</v>
-      </c>
-      <c r="L19" s="6">
+      <c r="K19" s="4">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
         <v>16.78</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="4">
         <v>16.25</v>
       </c>
-      <c r="N19" s="6">
-        <v>1</v>
-      </c>
-      <c r="O19" s="6">
+      <c r="N19" s="4">
+        <v>1</v>
+      </c>
+      <c r="O19" s="4">
         <v>3</v>
       </c>
-      <c r="P19" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="6">
+      <c r="P19" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R19" s="6">
+      <c r="R19" s="4">
         <v>3.33</v>
       </c>
-      <c r="S19" s="6">
+      <c r="S19" s="4">
         <v>0.3</v>
       </c>
-      <c r="T19" s="6">
+      <c r="T19" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U19" s="6">
+      <c r="U19" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V19" s="6">
+      <c r="V19" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W19" s="6">
+      <c r="W19" s="4">
         <v>16477</v>
       </c>
-      <c r="X19" s="6"/>
+      <c r="X19" s="4"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="4">
         <v>150</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="4">
         <v>0.23</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="4">
         <v>-9.26</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="4">
         <v>0.2</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L20" s="4">
         <v>15.65</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="4">
         <v>15.18</v>
       </c>
-      <c r="N20" s="6">
-        <v>1</v>
-      </c>
-      <c r="O20" s="6">
+      <c r="N20" s="4">
+        <v>1</v>
+      </c>
+      <c r="O20" s="4">
         <v>3</v>
       </c>
-      <c r="P20" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="6">
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R20" s="6">
+      <c r="R20" s="4">
         <v>3.46</v>
       </c>
-      <c r="S20" s="6">
+      <c r="S20" s="4">
         <v>0.3</v>
       </c>
-      <c r="T20" s="6">
+      <c r="T20" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U20" s="6">
+      <c r="U20" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V20" s="6">
+      <c r="V20" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W20" s="6">
+      <c r="W20" s="4">
         <v>16477</v>
       </c>
-      <c r="X20" s="6"/>
+      <c r="X20" s="4"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="4">
         <v>150</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="4">
         <v>0.42</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="4">
         <v>-9.06</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="4">
         <v>0.5</v>
       </c>
-      <c r="L21" s="6">
+      <c r="L21" s="4">
         <v>14.03</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="4">
         <v>13.54</v>
       </c>
-      <c r="N21" s="6">
-        <v>1</v>
-      </c>
-      <c r="O21" s="6">
+      <c r="N21" s="4">
+        <v>1</v>
+      </c>
+      <c r="O21" s="4">
         <v>4</v>
       </c>
-      <c r="P21" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="6">
+      <c r="P21" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R21" s="6">
+      <c r="R21" s="4">
         <v>4.9400000000000004</v>
       </c>
-      <c r="S21" s="6">
+      <c r="S21" s="4">
         <v>0.32</v>
       </c>
-      <c r="T21" s="6">
+      <c r="T21" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U21" s="6">
+      <c r="U21" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V21" s="6">
+      <c r="V21" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="W21" s="6">
+      <c r="W21" s="4">
         <v>16476</v>
       </c>
-      <c r="X21" s="6"/>
+      <c r="X21" s="4"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="4">
         <v>150</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="4">
         <v>-8.5399999999999991</v>
       </c>
-      <c r="K22" s="6">
-        <v>1</v>
-      </c>
-      <c r="L22" s="6">
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
         <v>15.41</v>
       </c>
-      <c r="M22" s="6">
+      <c r="M22" s="4">
         <v>15</v>
       </c>
-      <c r="N22" s="6">
-        <v>1</v>
-      </c>
-      <c r="O22" s="6">
+      <c r="N22" s="4">
+        <v>1</v>
+      </c>
+      <c r="O22" s="4">
         <v>4</v>
       </c>
-      <c r="P22" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="6">
+      <c r="P22" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R22" s="6">
+      <c r="R22" s="4">
         <v>6.62</v>
       </c>
-      <c r="S22" s="6">
+      <c r="S22" s="4">
         <v>0.32</v>
       </c>
-      <c r="T22" s="6">
+      <c r="T22" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="U22" s="6">
+      <c r="U22" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V22" s="6">
+      <c r="V22" s="4">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="W22" s="6">
+      <c r="W22" s="4">
         <v>16477</v>
       </c>
-      <c r="X22" s="6"/>
+      <c r="X22" s="4"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -4955,594 +4949,602 @@
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="4">
         <v>160</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="4">
         <v>0.16</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="4">
         <v>-9.2799999999999994</v>
       </c>
-      <c r="K24" s="6">
-        <v>0</v>
-      </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6">
-        <v>1</v>
-      </c>
-      <c r="O24" s="6">
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4">
+        <v>1</v>
+      </c>
+      <c r="O24" s="4">
         <v>2</v>
       </c>
-      <c r="P24" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="6">
+      <c r="P24" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R24" s="6">
+      <c r="R24" s="4">
         <v>2.57</v>
       </c>
-      <c r="S24" s="6">
+      <c r="S24" s="4">
         <v>0.28000000000000003</v>
       </c>
-      <c r="T24" s="6">
+      <c r="T24" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="U24" s="6">
+      <c r="U24" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V24" s="6">
+      <c r="V24" s="4">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="W24" s="6">
+      <c r="W24" s="4">
         <v>16478</v>
       </c>
-      <c r="X24" s="6"/>
+      <c r="X24" s="4"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="4">
         <v>200</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="4">
         <v>0.47</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="4">
         <v>-9.1199999999999992</v>
       </c>
-      <c r="K25" s="6">
-        <v>0</v>
-      </c>
-      <c r="L25" s="6">
+      <c r="K25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25" s="4">
         <v>14.27</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="4">
         <v>13.98</v>
       </c>
-      <c r="N25" s="6">
-        <v>1</v>
-      </c>
-      <c r="O25" s="6">
+      <c r="N25" s="4">
+        <v>1</v>
+      </c>
+      <c r="O25" s="4">
         <v>2</v>
       </c>
-      <c r="P25" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="6">
+      <c r="P25" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R25" s="4">
         <v>2.89</v>
       </c>
-      <c r="S25" s="6">
+      <c r="S25" s="4">
         <v>0.3</v>
       </c>
-      <c r="T25" s="6">
+      <c r="T25" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="U25" s="6">
+      <c r="U25" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V25" s="6">
+      <c r="V25" s="4">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="W25" s="6">
+      <c r="W25" s="4">
         <v>16479</v>
       </c>
-      <c r="X25" s="6"/>
+      <c r="X25" s="4"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="4">
         <v>150</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="4">
         <v>0.41</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="4">
         <v>-9.19</v>
       </c>
-      <c r="K26" s="6">
-        <v>0</v>
-      </c>
-      <c r="L26" s="6">
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
         <v>15.05</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="4">
         <v>14.71</v>
       </c>
-      <c r="N26" s="6">
-        <v>1</v>
-      </c>
-      <c r="O26" s="6">
+      <c r="N26" s="4">
+        <v>1</v>
+      </c>
+      <c r="O26" s="4">
         <v>2</v>
       </c>
-      <c r="P26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="6">
+      <c r="P26" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R26" s="6">
+      <c r="R26" s="4">
         <v>2.0299999999999998</v>
       </c>
-      <c r="S26" s="6">
+      <c r="S26" s="4">
         <v>0.26</v>
       </c>
-      <c r="T26" s="6">
+      <c r="T26" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U26" s="6">
+      <c r="U26" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V26" s="6">
+      <c r="V26" s="4">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="W26" s="6">
+      <c r="W26" s="4">
         <v>16479</v>
       </c>
-      <c r="X26" s="6"/>
+      <c r="X26" s="4"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="4">
         <v>160</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="4">
         <v>0.17</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="4">
         <v>-9.34</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="4">
         <v>0.1</v>
       </c>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6">
-        <v>1</v>
-      </c>
-      <c r="O27" s="6">
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4">
+        <v>1</v>
+      </c>
+      <c r="O27" s="4">
         <v>3</v>
       </c>
-      <c r="P27" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="6">
+      <c r="P27" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R27" s="6">
+      <c r="R27" s="4">
         <v>3.52</v>
       </c>
-      <c r="S27" s="6">
+      <c r="S27" s="4">
         <v>0.31</v>
       </c>
-      <c r="T27" s="6">
+      <c r="T27" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U27" s="6">
+      <c r="U27" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V27" s="6">
+      <c r="V27" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W27" s="6">
+      <c r="W27" s="4">
         <v>16478</v>
       </c>
-      <c r="X27" s="6"/>
+      <c r="X27" s="4"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="4">
         <v>150</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="H28" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="4">
         <v>0.2</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28" s="4">
         <v>-9.81</v>
       </c>
-      <c r="K28" s="6">
-        <v>0</v>
-      </c>
-      <c r="L28" s="6">
+      <c r="K28" s="4">
+        <v>0</v>
+      </c>
+      <c r="L28" s="4">
         <v>16.57</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M28" s="4">
         <v>15.85</v>
       </c>
-      <c r="N28" s="6">
-        <v>1</v>
-      </c>
-      <c r="O28" s="6">
+      <c r="N28" s="4">
+        <v>1</v>
+      </c>
+      <c r="O28" s="4">
         <v>4</v>
       </c>
-      <c r="P28" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="6">
+      <c r="P28" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R28" s="6">
+      <c r="R28" s="4">
         <v>5.56</v>
       </c>
-      <c r="S28" s="6">
+      <c r="S28" s="4">
         <v>0.38</v>
       </c>
-      <c r="T28" s="6">
+      <c r="T28" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="U28" s="6">
+      <c r="U28" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V28" s="6">
+      <c r="V28" s="4">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="W28" s="6">
+      <c r="W28" s="4">
         <v>16479</v>
       </c>
-      <c r="X28" s="6"/>
+      <c r="X28" s="4"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="7">
         <v>160</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="7">
         <v>0.3</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="7">
         <v>-7.96</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="7">
         <v>1.2</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="7">
         <v>15.63</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="7">
         <v>15.48</v>
       </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-      <c r="O29">
+      <c r="N29" s="7">
+        <v>1</v>
+      </c>
+      <c r="O29" s="7">
         <v>6</v>
       </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="Q29">
+      <c r="P29" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="7">
         <v>11.33</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="7">
         <v>0.36</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="7">
         <v>6</v>
       </c>
-      <c r="U29">
+      <c r="U29" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V29">
+      <c r="V29" s="7">
         <v>7</v>
       </c>
+      <c r="W29" s="7">
+        <v>16598</v>
+      </c>
+      <c r="X29" s="7"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="4">
         <v>200</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="4">
         <v>0.16</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="4">
         <v>-8.94</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K30" s="4">
         <v>0.6</v>
       </c>
-      <c r="L30" s="6">
+      <c r="L30" s="4">
         <v>17.79</v>
       </c>
-      <c r="M30" s="6">
+      <c r="M30" s="4">
         <v>17.32</v>
       </c>
-      <c r="N30" s="6">
-        <v>1</v>
-      </c>
-      <c r="O30" s="6">
+      <c r="N30" s="4">
+        <v>1</v>
+      </c>
+      <c r="O30" s="4">
         <v>6</v>
       </c>
-      <c r="P30" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="6">
+      <c r="P30" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="R30" s="6">
+      <c r="R30" s="4">
         <v>8.7100000000000009</v>
       </c>
-      <c r="S30" s="6">
+      <c r="S30" s="4">
         <v>0.42</v>
       </c>
-      <c r="T30" s="6">
+      <c r="T30" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="U30" s="6">
+      <c r="U30" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V30" s="6">
+      <c r="V30" s="4">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="W30" s="6">
+      <c r="W30" s="4">
         <v>16479</v>
       </c>
-      <c r="X30" s="6"/>
+      <c r="X30" s="4"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="7">
         <v>160</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="7">
         <v>0.49</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="7">
         <v>-7.33</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="7">
         <v>1.2</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="7">
         <v>12.71</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="7">
         <v>12.94</v>
       </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-      <c r="O31">
+      <c r="N31" s="7">
+        <v>1</v>
+      </c>
+      <c r="O31" s="7">
         <v>7</v>
       </c>
-      <c r="P31">
-        <v>1</v>
-      </c>
-      <c r="Q31">
+      <c r="P31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="7">
         <v>12.38</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="7">
         <v>0.22</v>
       </c>
-      <c r="T31">
+      <c r="T31" s="7">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="U31">
+      <c r="U31" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="7">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
+      <c r="W31" s="7">
+        <v>16597</v>
+      </c>
+      <c r="X31" s="7"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -5686,224 +5688,228 @@
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G34" s="7">
         <v>94</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="7">
         <v>0.15</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="7">
         <v>-9.89</v>
       </c>
-      <c r="K34" s="3">
-        <v>0</v>
-      </c>
-      <c r="L34" s="3">
+      <c r="K34" s="7">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7">
         <v>15.96</v>
       </c>
-      <c r="M34" s="3">
+      <c r="M34" s="7">
         <v>15.2</v>
       </c>
-      <c r="N34" s="3">
-        <v>1</v>
-      </c>
-      <c r="O34" s="3">
+      <c r="N34" s="7">
+        <v>1</v>
+      </c>
+      <c r="O34" s="7">
         <v>2</v>
       </c>
-      <c r="P34" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="3">
+      <c r="P34" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R34" s="3">
+      <c r="R34" s="7">
         <v>2.8</v>
       </c>
-      <c r="S34" s="3">
+      <c r="S34" s="7">
         <v>0.27</v>
       </c>
-      <c r="T34" s="3">
-        <v>1</v>
-      </c>
-      <c r="U34" s="3">
+      <c r="T34" s="7">
+        <v>1</v>
+      </c>
+      <c r="U34" s="7">
         <v>2</v>
       </c>
-      <c r="V34" s="3">
+      <c r="V34" s="7">
         <f>Q34</f>
         <v>3</v>
       </c>
-      <c r="W34" s="3"/>
-      <c r="X34" s="3"/>
+      <c r="W34" s="7">
+        <v>16595</v>
+      </c>
+      <c r="X34" s="7"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="7">
         <v>94</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="7">
         <v>0.15</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="7">
         <v>-9.92</v>
       </c>
-      <c r="K35" s="3">
-        <v>0</v>
-      </c>
-      <c r="L35" s="3">
+      <c r="K35" s="7">
+        <v>0</v>
+      </c>
+      <c r="L35" s="7">
         <v>15.78</v>
       </c>
-      <c r="M35" s="3">
+      <c r="M35" s="7">
         <v>15</v>
       </c>
-      <c r="N35" s="3">
-        <v>1</v>
-      </c>
-      <c r="O35" s="3">
+      <c r="N35" s="7">
+        <v>1</v>
+      </c>
+      <c r="O35" s="7">
         <v>2</v>
       </c>
-      <c r="P35" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="3">
+      <c r="P35" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R35" s="3">
+      <c r="R35" s="7">
         <v>2.94</v>
       </c>
-      <c r="S35" s="3">
+      <c r="S35" s="7">
         <v>0.27</v>
       </c>
-      <c r="T35" s="3">
-        <v>1</v>
-      </c>
-      <c r="U35" s="3">
+      <c r="T35" s="7">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7">
         <v>2</v>
       </c>
-      <c r="V35" s="3">
+      <c r="V35" s="7">
         <f t="shared" ref="V35:V36" si="5">Q35</f>
         <v>3</v>
       </c>
-      <c r="W35" s="3"/>
-      <c r="X35" s="3"/>
+      <c r="W35" s="7">
+        <v>16595</v>
+      </c>
+      <c r="X35" s="7"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="4">
         <v>94</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="4">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="J36" s="6">
+      <c r="J36" s="4">
         <v>-10.18</v>
       </c>
-      <c r="K36" s="6">
-        <v>0</v>
-      </c>
-      <c r="L36" s="6">
+      <c r="K36" s="4">
+        <v>0</v>
+      </c>
+      <c r="L36" s="4">
         <v>19.34</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36" s="4">
         <v>18.399999999999999</v>
       </c>
-      <c r="N36" s="6">
-        <v>1</v>
-      </c>
-      <c r="O36" s="6">
+      <c r="N36" s="4">
+        <v>1</v>
+      </c>
+      <c r="O36" s="4">
         <v>3</v>
       </c>
-      <c r="P36" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="6">
+      <c r="P36" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R36" s="6">
+      <c r="R36" s="4">
         <v>4.57</v>
       </c>
-      <c r="S36" s="6">
+      <c r="S36" s="4">
         <v>0.32</v>
       </c>
-      <c r="T36" s="6">
+      <c r="T36" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U36" s="6">
+      <c r="U36" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V36" s="6">
+      <c r="V36" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="W36" s="6">
+      <c r="W36" s="4">
         <v>16480</v>
       </c>
-      <c r="X36" s="6"/>
+      <c r="X36" s="4"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -6054,370 +6060,373 @@
       <c r="X38" s="2"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="6">
         <v>160</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="6">
         <v>0.19</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="6">
         <v>-8.9499999999999993</v>
       </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>1</v>
-      </c>
-      <c r="O39">
-        <v>1</v>
-      </c>
-      <c r="P39">
-        <v>1</v>
-      </c>
-      <c r="Q39">
+      <c r="K39" s="6">
+        <v>0</v>
+      </c>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6">
+        <v>1</v>
+      </c>
+      <c r="O39" s="6">
+        <v>1</v>
+      </c>
+      <c r="P39" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="6">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="6">
         <v>1.6</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="6">
         <v>0.24</v>
       </c>
-      <c r="T39">
+      <c r="T39" s="6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U39">
+      <c r="U39" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V39">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
+      <c r="V39" s="6">
+        <v>0</v>
+      </c>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="4">
         <v>160</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J40" s="6">
+      <c r="J40" s="4">
         <v>-8.7100000000000009</v>
       </c>
-      <c r="K40" s="6">
+      <c r="K40" s="4">
         <v>0.4</v>
       </c>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6">
-        <v>1</v>
-      </c>
-      <c r="O40" s="6">
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4">
+        <v>1</v>
+      </c>
+      <c r="O40" s="4">
         <v>2</v>
       </c>
-      <c r="P40" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="6">
+      <c r="P40" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="R40" s="6">
+      <c r="R40" s="4">
         <v>2.4700000000000002</v>
       </c>
-      <c r="S40" s="6">
+      <c r="S40" s="4">
         <v>0.26</v>
       </c>
-      <c r="T40" s="6">
+      <c r="T40" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="U40" s="6">
+      <c r="U40" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V40" s="6">
+      <c r="V40" s="4">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="W40" s="6">
+      <c r="W40" s="4">
         <v>16481</v>
       </c>
-      <c r="X40" s="6"/>
+      <c r="X40" s="4"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="4">
         <v>160</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="4">
         <v>1.25</v>
       </c>
-      <c r="J41" s="6">
+      <c r="J41" s="4">
         <v>-8.09</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K41" s="4">
         <v>0.8</v>
       </c>
-      <c r="L41" s="6">
+      <c r="L41" s="4">
         <v>12</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41" s="4">
         <v>11.96</v>
       </c>
-      <c r="N41" s="6">
-        <v>1</v>
-      </c>
-      <c r="O41" s="6">
+      <c r="N41" s="4">
+        <v>1</v>
+      </c>
+      <c r="O41" s="4">
         <v>3</v>
       </c>
-      <c r="P41" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="6">
+      <c r="P41" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R41" s="6">
+      <c r="R41" s="4">
         <v>4.8099999999999996</v>
       </c>
-      <c r="S41" s="6">
+      <c r="S41" s="4">
         <v>0.3</v>
       </c>
-      <c r="T41" s="6">
+      <c r="T41" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U41" s="6">
+      <c r="U41" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V41" s="6">
+      <c r="V41" s="4">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="W41" s="6">
+      <c r="W41" s="4">
         <v>16482</v>
       </c>
-      <c r="X41" s="6"/>
+      <c r="X41" s="4"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="4">
         <v>160</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H42" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42" s="4">
         <v>0.51</v>
       </c>
-      <c r="J42" s="6">
+      <c r="J42" s="4">
         <v>-8.09</v>
       </c>
-      <c r="K42" s="6">
+      <c r="K42" s="4">
         <v>0.7</v>
       </c>
-      <c r="L42" s="6">
+      <c r="L42" s="4">
         <v>13.5</v>
       </c>
-      <c r="M42" s="6">
+      <c r="M42" s="4">
         <v>13.5</v>
       </c>
-      <c r="N42" s="6">
-        <v>1</v>
-      </c>
-      <c r="O42" s="6">
+      <c r="N42" s="4">
+        <v>1</v>
+      </c>
+      <c r="O42" s="4">
         <v>3</v>
       </c>
-      <c r="P42" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q42" s="6">
+      <c r="P42" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R42" s="6">
+      <c r="R42" s="4">
         <v>3.7</v>
       </c>
-      <c r="S42" s="6">
+      <c r="S42" s="4">
         <v>0.28000000000000003</v>
       </c>
-      <c r="T42" s="6">
+      <c r="T42" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U42" s="6">
+      <c r="U42" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V42" s="6">
+      <c r="V42" s="4">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="W42" s="6">
+      <c r="W42" s="4">
         <v>16482</v>
       </c>
-      <c r="X42" s="6" t="s">
+      <c r="X42" s="4" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="4">
         <v>160</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43" s="4">
         <v>0.19</v>
       </c>
-      <c r="J43" s="6">
+      <c r="J43" s="4">
         <v>-8.6999999999999993</v>
       </c>
-      <c r="K43" s="6">
+      <c r="K43" s="4">
         <v>0.8</v>
       </c>
-      <c r="L43" s="6">
+      <c r="L43" s="4">
         <v>16.670000000000002</v>
       </c>
-      <c r="M43" s="6">
+      <c r="M43" s="4">
         <v>16.25</v>
       </c>
-      <c r="N43" s="6">
-        <v>1</v>
-      </c>
-      <c r="O43" s="6">
+      <c r="N43" s="4">
+        <v>1</v>
+      </c>
+      <c r="O43" s="4">
         <v>4</v>
       </c>
-      <c r="P43" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="6">
+      <c r="P43" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="R43" s="6">
+      <c r="R43" s="4">
         <v>6.08</v>
       </c>
-      <c r="S43" s="6">
+      <c r="S43" s="4">
         <v>0.32</v>
       </c>
-      <c r="T43" s="6">
+      <c r="T43" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="U43" s="6">
+      <c r="U43" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V43" s="6">
+      <c r="V43" s="4">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="W43" s="6">
+      <c r="W43" s="4">
         <v>16481</v>
       </c>
-      <c r="X43" s="6"/>
+      <c r="X43" s="4"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -6492,80 +6501,80 @@
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="4">
         <v>160</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I45" s="4">
         <v>0.25</v>
       </c>
-      <c r="J45" s="6">
+      <c r="J45" s="4">
         <v>-7.41</v>
       </c>
-      <c r="K45" s="6">
-        <v>1</v>
-      </c>
-      <c r="L45" s="6">
+      <c r="K45" s="4">
+        <v>1</v>
+      </c>
+      <c r="L45" s="4">
         <v>15</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45" s="4">
         <v>15.28</v>
       </c>
-      <c r="N45" s="6">
-        <v>1</v>
-      </c>
-      <c r="O45" s="6">
+      <c r="N45" s="4">
+        <v>1</v>
+      </c>
+      <c r="O45" s="4">
         <v>5</v>
       </c>
-      <c r="P45" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="6">
+      <c r="P45" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R45" s="6">
+      <c r="R45" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="S45" s="6">
+      <c r="S45" s="4">
         <v>0.21</v>
       </c>
-      <c r="T45" s="6">
+      <c r="T45" s="4">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="U45" s="6">
+      <c r="U45" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V45" s="6">
+      <c r="V45" s="4">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="W45" s="6">
+      <c r="W45" s="4">
         <v>16481</v>
       </c>
-      <c r="X45" s="6"/>
+      <c r="X45" s="4"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -6640,222 +6649,235 @@
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="7">
         <v>160</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="7">
         <v>0.78</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="7">
         <v>-9.41</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="7">
         <v>0.5</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="7">
         <v>14.51</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="7">
         <v>13.8</v>
       </c>
-      <c r="N47">
-        <v>1</v>
-      </c>
-      <c r="O47">
+      <c r="N47" s="7">
+        <v>1</v>
+      </c>
+      <c r="O47" s="7">
         <v>7</v>
       </c>
-      <c r="P47">
-        <v>1</v>
-      </c>
-      <c r="Q47">
+      <c r="P47" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R47">
+      <c r="R47" s="7">
         <v>10.58</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="7">
         <v>0.45</v>
       </c>
-      <c r="T47">
+      <c r="T47" s="7">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="U47">
+      <c r="U47" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V47">
+      <c r="V47" s="7">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
+      <c r="W47" s="7">
+        <v>16596</v>
+      </c>
+      <c r="X47" s="7"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="7">
         <v>160</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H48" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="7">
         <v>2.08</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="7">
         <v>-7.63</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="7">
         <v>1.5</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="7">
         <v>11.02</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="7">
         <v>10.93</v>
       </c>
-      <c r="N48">
-        <v>1</v>
-      </c>
-      <c r="O48">
+      <c r="N48" s="7">
+        <v>1</v>
+      </c>
+      <c r="O48" s="7">
         <v>7</v>
       </c>
-      <c r="P48">
-        <v>1</v>
-      </c>
-      <c r="Q48">
+      <c r="P48" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R48">
+      <c r="R48" s="7">
         <v>13.6</v>
       </c>
-      <c r="S48">
+      <c r="S48" s="7">
         <v>0.34</v>
       </c>
-      <c r="T48">
+      <c r="T48" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="U48">
+      <c r="U48" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V48">
+      <c r="V48" s="7">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
+      <c r="W48" s="7">
+        <v>16597</v>
+      </c>
+      <c r="X48" s="7"/>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="7">
         <v>114</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="7">
         <v>0.9</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="7">
         <v>-9.07</v>
       </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49">
+      <c r="K49" s="7">
+        <v>1</v>
+      </c>
+      <c r="L49" s="7">
         <v>12.82</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="7">
         <v>12.08</v>
       </c>
-      <c r="N49">
-        <v>1</v>
-      </c>
-      <c r="O49">
+      <c r="N49" s="7">
+        <v>1</v>
+      </c>
+      <c r="O49" s="7">
         <v>7</v>
       </c>
-      <c r="P49">
-        <v>1</v>
-      </c>
-      <c r="Q49">
+      <c r="P49" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="R49">
+      <c r="R49" s="7">
         <v>10.6</v>
       </c>
-      <c r="S49">
+      <c r="S49" s="7">
         <v>0.36</v>
       </c>
-      <c r="T49">
+      <c r="T49" s="7">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="U49">
+      <c r="U49" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V49">
+      <c r="V49" s="7">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
+      <c r="W49" s="7">
+        <v>16599</v>
+      </c>
+      <c r="X49" s="7"/>
+      <c r="Y49" s="7"/>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>375</v>
       </c>
@@ -6927,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>259</v>
       </c>
@@ -6999,7 +7021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>264</v>
       </c>
@@ -7071,7 +7093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>269</v>
       </c>
@@ -7143,7 +7165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>275</v>
       </c>
@@ -7212,7 +7234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>279</v>
       </c>
@@ -7284,7 +7306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>285</v>
       </c>
@@ -7356,7 +7378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -7428,7 +7450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>297</v>
       </c>
@@ -7500,7 +7522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>302</v>
       </c>
@@ -7572,7 +7594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>307</v>
       </c>
@@ -7644,7 +7666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>312</v>
       </c>
@@ -7716,7 +7738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>317</v>
       </c>
@@ -7788,7 +7810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>322</v>
       </c>
@@ -7860,7 +7882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>327</v>
       </c>
@@ -8133,7 +8155,7 @@
         <v>0.48</v>
       </c>
       <c r="T67">
-        <f t="shared" ref="T67:T69" si="8">ROUND(R67+0.3,0)</f>
+        <f t="shared" ref="T67:T68" si="8">ROUND(R67+0.3,0)</f>
         <v>13</v>
       </c>
       <c r="U67">
@@ -8218,205 +8240,222 @@
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="A69" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="7">
         <v>385</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="7">
         <v>0.754</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="7">
         <v>-8.5399999999999991</v>
       </c>
-      <c r="K69">
-        <v>0</v>
-      </c>
-      <c r="L69">
+      <c r="K69" s="7">
+        <v>0</v>
+      </c>
+      <c r="L69" s="7">
         <v>14.1</v>
       </c>
-      <c r="M69">
+      <c r="M69" s="7">
         <v>14.16</v>
       </c>
-      <c r="N69">
-        <v>1</v>
-      </c>
-      <c r="O69">
+      <c r="N69" s="7">
+        <v>1</v>
+      </c>
+      <c r="O69" s="7">
         <v>3</v>
       </c>
-      <c r="P69">
-        <v>1</v>
-      </c>
-      <c r="Q69">
+      <c r="P69" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="7">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="R69">
+      <c r="R69" s="7">
         <v>3.49</v>
       </c>
-      <c r="S69">
+      <c r="S69" s="7">
         <v>0.36</v>
       </c>
-      <c r="T69">
+      <c r="T69" s="7">
         <v>3</v>
       </c>
-      <c r="U69">
+      <c r="U69" s="7">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="V69">
+      <c r="V69" s="7">
         <f t="shared" ref="V69" si="11">O69+P69</f>
         <v>4</v>
       </c>
+      <c r="W69" s="7">
+        <v>16594</v>
+      </c>
+      <c r="X69" s="7"/>
+      <c r="Y69" s="7"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="7" t="s">
         <v>382</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="7">
         <v>140</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="7">
         <v>1.4</v>
       </c>
-      <c r="J70">
+      <c r="J70" s="7">
         <v>-9.52</v>
       </c>
-      <c r="K70">
+      <c r="K70" s="7">
         <v>0.3</v>
       </c>
-      <c r="M70">
+      <c r="L70" s="7"/>
+      <c r="M70" s="7">
         <v>10.86</v>
       </c>
-      <c r="N70">
-        <v>1</v>
-      </c>
-      <c r="O70">
-        <v>0</v>
-      </c>
-      <c r="P70">
-        <v>0</v>
-      </c>
-      <c r="Q70">
-        <v>0</v>
-      </c>
-      <c r="R70">
-        <v>0</v>
-      </c>
-      <c r="S70">
+      <c r="N70" s="7">
+        <v>1</v>
+      </c>
+      <c r="O70" s="7">
+        <v>0</v>
+      </c>
+      <c r="P70" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="7">
+        <v>0</v>
+      </c>
+      <c r="R70" s="7">
+        <v>0</v>
+      </c>
+      <c r="S70" s="7">
         <v>2</v>
       </c>
-      <c r="T70">
+      <c r="T70" s="7">
         <v>2</v>
       </c>
-      <c r="U70">
-        <v>1</v>
-      </c>
-      <c r="V70">
+      <c r="U70" s="7">
+        <v>1</v>
+      </c>
+      <c r="V70" s="7">
         <v>3</v>
       </c>
+      <c r="W70" s="7">
+        <v>16593</v>
+      </c>
+      <c r="X70" s="7"/>
+      <c r="Y70" s="7"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="A71" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="7">
         <v>94</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H71" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I71">
+      <c r="I71" s="7">
         <v>0.3</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="7">
         <v>-10.6</v>
       </c>
-      <c r="K71">
-        <v>0</v>
-      </c>
-      <c r="M71">
+      <c r="K71" s="7">
+        <v>0</v>
+      </c>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7">
         <v>14.1</v>
       </c>
-      <c r="N71">
-        <v>1</v>
-      </c>
-      <c r="O71">
-        <v>0</v>
-      </c>
-      <c r="P71">
-        <v>0</v>
-      </c>
-      <c r="Q71">
-        <v>0</v>
-      </c>
-      <c r="R71">
-        <v>0</v>
-      </c>
-      <c r="S71">
+      <c r="N71" s="7">
+        <v>1</v>
+      </c>
+      <c r="O71" s="7">
+        <v>0</v>
+      </c>
+      <c r="P71" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="7">
+        <v>0</v>
+      </c>
+      <c r="R71" s="7">
+        <v>0</v>
+      </c>
+      <c r="S71" s="7">
         <v>8</v>
       </c>
-      <c r="T71">
-        <v>0</v>
-      </c>
-      <c r="U71">
+      <c r="T71" s="7">
+        <v>0</v>
+      </c>
+      <c r="U71" s="7">
         <v>8</v>
       </c>
-      <c r="V71">
+      <c r="V71" s="7">
         <v>8</v>
       </c>
+      <c r="W71" s="7">
+        <v>16596</v>
+      </c>
+      <c r="X71" s="7"/>
+      <c r="Y71" s="7"/>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -9269,7 +9308,7 @@
       <c r="A83" t="s">
         <v>469</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="5" t="s">
         <v>470</v>
       </c>
       <c r="C83" t="s">
@@ -9278,7 +9317,7 @@
       <c r="D83" t="s">
         <v>472</v>
       </c>
-      <c r="E83" s="4" t="s">
+      <c r="E83" s="3" t="s">
         <v>473</v>
       </c>
       <c r="F83" t="s">
@@ -9343,7 +9382,7 @@
       <c r="A84" t="s">
         <v>476</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B84" s="5" t="s">
         <v>477</v>
       </c>
       <c r="C84" t="s">
@@ -9352,7 +9391,7 @@
       <c r="D84" t="s">
         <v>479</v>
       </c>
-      <c r="E84" s="4" t="s">
+      <c r="E84" s="3" t="s">
         <v>480</v>
       </c>
       <c r="F84" t="s">
@@ -9420,7 +9459,7 @@
       <c r="D85" t="s">
         <v>485</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="3" t="s">
         <v>486</v>
       </c>
       <c r="F85" t="s">
@@ -9482,7 +9521,7 @@
       <c r="A86" t="s">
         <v>488</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B86" s="5" t="s">
         <v>489</v>
       </c>
       <c r="C86" t="s">
@@ -9491,7 +9530,7 @@
       <c r="D86" t="s">
         <v>491</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="3" t="s">
         <v>492</v>
       </c>
       <c r="F86" t="s">
@@ -9559,13 +9598,13 @@
       <c r="A87" t="s">
         <v>495</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B87" s="5" t="s">
         <v>496</v>
       </c>
       <c r="D87" t="s">
         <v>497</v>
       </c>
-      <c r="E87" s="4" t="s">
+      <c r="E87" s="3" t="s">
         <v>498</v>
       </c>
       <c r="F87" t="s">
@@ -9636,7 +9675,7 @@
       <c r="D88" t="s">
         <v>500</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="3" t="s">
         <v>501</v>
       </c>
       <c r="F88" t="s">
@@ -9698,7 +9737,7 @@
       <c r="A89" t="s">
         <v>504</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="5" t="s">
         <v>506</v>
       </c>
       <c r="C89" t="s">
@@ -9707,7 +9746,7 @@
       <c r="D89" t="s">
         <v>508</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E89" s="3" t="s">
         <v>509</v>
       </c>
       <c r="F89" t="s">
@@ -9775,7 +9814,7 @@
       <c r="A90" t="s">
         <v>510</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B90" s="5" t="s">
         <v>517</v>
       </c>
       <c r="C90" t="s">
@@ -9784,7 +9823,7 @@
       <c r="D90" t="s">
         <v>511</v>
       </c>
-      <c r="E90" s="4" t="s">
+      <c r="E90" s="3" t="s">
         <v>512</v>
       </c>
       <c r="F90" t="s">
@@ -9852,7 +9891,7 @@
       <c r="A91" t="s">
         <v>513</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B91" s="5" t="s">
         <v>515</v>
       </c>
       <c r="C91" t="s">
@@ -9931,7 +9970,7 @@
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72">
+  <conditionalFormatting sqref="A39:X68 V70:X70 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
     <cfRule type="expression" dxfId="68" priority="67">
       <formula>$N39=0</formula>
     </cfRule>
@@ -9939,7 +9978,7 @@
       <formula>"$N2=0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72">
+  <conditionalFormatting sqref="A39:U68 F70:F71 T70:T71 A71:C71 B70:C70 O72:W72 N72:N78 M70:S70 G71:S71 Y72 W71">
     <cfRule type="expression" dxfId="66" priority="69">
       <formula>$N$2=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated the number of orbits for recx5 and recx9 (16595 ended up needed 2 STIS orbits for each visit)
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA581FDD-9B00-8343-879E-ED9DCD2EE181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CCBAB6-DFEA-334F-9552-A1118E44689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="920" windowWidth="35780" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="920" windowWidth="35780" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
@@ -3164,8 +3164,8 @@
   <dimension ref="A1:Y91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W38" sqref="W38"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5747,14 +5747,13 @@
         <v>0.27</v>
       </c>
       <c r="T34" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U34" s="7">
         <v>2</v>
       </c>
       <c r="V34" s="7">
-        <f>Q34</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W34" s="7">
         <v>16595</v>
@@ -5821,14 +5820,13 @@
         <v>0.27</v>
       </c>
       <c r="T35" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U35" s="7">
         <v>2</v>
       </c>
       <c r="V35" s="7">
-        <f t="shared" ref="V35:V36" si="5">Q35</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W35" s="7">
         <v>16595</v>
@@ -5903,7 +5901,7 @@
         <v>1</v>
       </c>
       <c r="V36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="V35:V36" si="5">Q36</f>
         <v>4</v>
       </c>
       <c r="W36" s="4">

</xml_diff>

<commit_message>
Removed Sz112 from sample (to save orbits following increase in orbit request due to throughputs etc) and adjusted orbit allocation for HD104137E (Rachel's program)
</commit_message>
<xml_diff>
--- a/data/target_metadata/full_sample_CTTS.xlsx
+++ b/data/target_metadata/full_sample_CTTS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CCBAB6-DFEA-334F-9552-A1118E44689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F45E47-7C79-8340-ADCE-9011424652A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2620" yWindow="920" windowWidth="35780" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,15 @@
     <sheet name="updated_full_sample_newAV_newSN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3163,9 +3172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X36" sqref="X36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="108" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V53" sqref="V53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5901,7 +5910,7 @@
         <v>1</v>
       </c>
       <c r="V36" s="4">
-        <f t="shared" ref="V35:V36" si="5">Q36</f>
+        <f t="shared" ref="V36" si="5">Q36</f>
         <v>4</v>
       </c>
       <c r="W36" s="4">
@@ -6858,16 +6867,14 @@
         <v>0.36</v>
       </c>
       <c r="T49" s="7">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="U49" s="7">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V49" s="7">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="W49" s="7">
         <v>16599</v>
@@ -7849,7 +7856,7 @@
         <v>15.39</v>
       </c>
       <c r="N63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O63">
         <v>5</v>
@@ -7877,7 +7884,7 @@
       </c>
       <c r="V63">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>